<commit_message>
Set All Model Load Orders
</commit_message>
<xml_diff>
--- a/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
+++ b/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
@@ -2542,7 +2542,7 @@
     </row>
     <row r="46" spans="1:16">
       <c r="A46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
         <v>16</v>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B50" t="s">
         <v>54</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="64" spans="1:16">
       <c r="A64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
         <v>54</v>
@@ -3779,7 +3779,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
         <v>77</v>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="110" spans="1:16">
       <c r="A110">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B110" t="s">
         <v>39</v>
@@ -5254,7 +5254,7 @@
     </row>
     <row r="114" spans="1:16">
       <c r="A114">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B114" t="s">
         <v>54</v>
@@ -5492,7 +5492,7 @@
     </row>
     <row r="120" spans="1:16">
       <c r="A120">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B120" t="s">
         <v>98</v>
@@ -6015,7 +6015,7 @@
     </row>
     <row r="133" spans="1:16">
       <c r="A133">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B133" t="s">
         <v>39</v>
@@ -6347,7 +6347,7 @@
     </row>
     <row r="141" spans="1:16">
       <c r="A141">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B141" t="s">
         <v>77</v>
@@ -6632,7 +6632,7 @@
     </row>
     <row r="148" spans="1:16">
       <c r="A148">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B148" t="s">
         <v>37</v>
@@ -7249,7 +7249,7 @@
     </row>
     <row r="163" spans="1:16">
       <c r="A163">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B163" t="s">
         <v>135</v>
@@ -7487,7 +7487,7 @@
     </row>
     <row r="169" spans="1:16">
       <c r="A169">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B169" t="s">
         <v>135</v>
@@ -7725,7 +7725,7 @@
     </row>
     <row r="175" spans="1:16">
       <c r="A175">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B175" t="s">
         <v>45</v>
@@ -7963,7 +7963,7 @@
     </row>
     <row r="181" spans="1:16">
       <c r="A181">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B181" t="s">
         <v>98</v>
@@ -8154,7 +8154,7 @@
     </row>
     <row r="186" spans="1:16">
       <c r="A186">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B186" t="s">
         <v>135</v>
@@ -8345,7 +8345,7 @@
     </row>
     <row r="191" spans="1:16">
       <c r="A191">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B191" t="s">
         <v>77</v>
@@ -8536,7 +8536,7 @@
     </row>
     <row r="196" spans="1:16">
       <c r="A196">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B196" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Prof Meeting 10/12 Changes
- Change Label to category
- Removed Assoc prefix from tables
- Database details now show db_name instead of model name
- Removed nulls from location
- Zipcode is now 10 digits long
</commit_message>
<xml_diff>
--- a/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
+++ b/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="157">
   <si>
     <t>Load Order</t>
   </si>
@@ -67,7 +67,7 @@
     <t>Rebecca Hutchinson</t>
   </si>
   <si>
-    <t>CustomerLabel</t>
+    <t>CustomerCategory</t>
   </si>
   <si>
     <t>id</t>
@@ -100,7 +100,7 @@
     <t>Kyle Dela Pena</t>
   </si>
   <si>
-    <t>EmployeeLabel</t>
+    <t>EmployeeCategory</t>
   </si>
   <si>
     <t>Alanna Gilcrease</t>
@@ -109,7 +109,7 @@
     <t>EmployeeStatus</t>
   </si>
   <si>
-    <t>Used to soft delete rows with a reason name and desc</t>
+    <t>Defines whether an employee is currently active or inactive</t>
   </si>
   <si>
     <t>status_name</t>
@@ -133,28 +133,40 @@
     <t>CustomerStatus</t>
   </si>
   <si>
+    <t>Describes the current relationship between the customer and the business (are they an Active customer? are they an inactive customer?)</t>
+  </si>
+  <si>
     <t>Srijana Shrestha</t>
   </si>
   <si>
     <t>ProductStatus</t>
   </si>
   <si>
+    <t>Refers to whether a product is available or not. Not that it is unavailable but also if it is not offered anymore</t>
+  </si>
+  <si>
     <t>StoreStatus</t>
   </si>
   <si>
+    <t>Soft delete of store.</t>
+  </si>
+  <si>
     <t>RewardStatus</t>
   </si>
   <si>
+    <t>Defines whether a particular reward is active/inactive. Primary attributes: active, inactive</t>
+  </si>
+  <si>
     <t>BanType</t>
   </si>
   <si>
-    <t>Describes why a type of product is banned</t>
+    <t>Describes why a specific product that is banned</t>
   </si>
   <si>
     <t>Jade Nguyen</t>
   </si>
   <si>
-    <t>PointReason</t>
+    <t>PointLogType</t>
   </si>
   <si>
     <t>Describes why points were added or removed</t>
@@ -163,15 +175,18 @@
     <t>Country</t>
   </si>
   <si>
+    <t>The nation that a particular entity (a store, a customer) is located in.</t>
+  </si>
+  <si>
+    <t>country_name</t>
+  </si>
+  <si>
+    <t>StateProvince</t>
+  </si>
+  <si>
     <t>Blank Description</t>
   </si>
   <si>
-    <t>country_name</t>
-  </si>
-  <si>
-    <t>StateProvince</t>
-  </si>
-  <si>
     <t>state_name</t>
   </si>
   <si>
@@ -202,6 +217,9 @@
     <t>Tier</t>
   </si>
   <si>
+    <t>Categories that loyalty customers are a part of based on number of points accummulated over time. Tiers such as bronze, silver, and gold tier for example.</t>
+  </si>
+  <si>
     <t>EmployeeType</t>
   </si>
   <si>
@@ -271,7 +289,7 @@
     <t>job_desc</t>
   </si>
   <si>
-    <t>AssocEmployeeLabel</t>
+    <t>EmployeeEmployeeCategory</t>
   </si>
   <si>
     <t>employee_id</t>
@@ -280,7 +298,7 @@
     <t>employee_label_id</t>
   </si>
   <si>
-    <t>AssocCustomerLabel</t>
+    <t>CustomerCustomerCategory</t>
   </si>
   <si>
     <t>customer_id</t>
@@ -445,7 +463,7 @@
     <t>product_assigned</t>
   </si>
   <si>
-    <t>StoreReward</t>
+    <t>Store Reward</t>
   </si>
   <si>
     <t>reward_id</t>
@@ -831,7 +849,7 @@
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
@@ -1426,7 +1444,7 @@
         <v>21</v>
       </c>
       <c r="P15" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1578,10 +1596,10 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
@@ -1620,7 +1638,7 @@
         <v>21</v>
       </c>
       <c r="P20" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1775,7 +1793,7 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -1814,7 +1832,7 @@
         <v>21</v>
       </c>
       <c r="P25" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1969,7 +1987,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
@@ -2008,7 +2026,7 @@
         <v>21</v>
       </c>
       <c r="P30" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2163,7 +2181,7 @@
         <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
@@ -2202,7 +2220,7 @@
         <v>21</v>
       </c>
       <c r="P35" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2304,10 +2322,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
         <v>18</v>
@@ -2346,7 +2364,7 @@
         <v>21</v>
       </c>
       <c r="P39" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -2451,7 +2469,7 @@
         <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -2490,7 +2508,7 @@
         <v>21</v>
       </c>
       <c r="P43" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -2504,7 +2522,7 @@
         <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
@@ -2548,7 +2566,7 @@
         <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
@@ -2587,7 +2605,7 @@
         <v>21</v>
       </c>
       <c r="P46" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -2601,7 +2619,7 @@
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
@@ -2648,7 +2666,7 @@
         <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E48" t="s">
         <v>19</v>
@@ -2689,10 +2707,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
@@ -2731,7 +2749,7 @@
         <v>21</v>
       </c>
       <c r="P50" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -2745,13 +2763,13 @@
         <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E51" t="s">
         <v>19</v>
       </c>
       <c r="F51">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G51" t="s">
         <v>25</v>
@@ -2763,10 +2781,10 @@
         <v>0</v>
       </c>
       <c r="J51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" t="b">
         <v>0</v>
@@ -2792,7 +2810,7 @@
         <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E52" t="s">
         <v>19</v>
@@ -2810,10 +2828,10 @@
         <v>0</v>
       </c>
       <c r="J52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L52" t="b">
         <v>0</v>
@@ -2839,7 +2857,7 @@
         <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E53" t="s">
         <v>19</v>
@@ -2857,10 +2875,10 @@
         <v>0</v>
       </c>
       <c r="J53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53" t="b">
         <v>0</v>
@@ -2886,7 +2904,7 @@
         <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
@@ -2930,7 +2948,7 @@
         <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D56" t="s">
         <v>18</v>
@@ -2969,7 +2987,7 @@
         <v>21</v>
       </c>
       <c r="P56" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -3074,7 +3092,7 @@
         <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
@@ -3215,10 +3233,10 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D64" t="s">
         <v>18</v>
@@ -3257,7 +3275,7 @@
         <v>21</v>
       </c>
       <c r="P64" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -3271,7 +3289,7 @@
         <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
@@ -3318,7 +3336,7 @@
         <v>23</v>
       </c>
       <c r="D66" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
@@ -3365,7 +3383,7 @@
         <v>23</v>
       </c>
       <c r="D67" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
@@ -3412,7 +3430,7 @@
         <v>23</v>
       </c>
       <c r="D68" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
@@ -3459,7 +3477,7 @@
         <v>23</v>
       </c>
       <c r="D69" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
@@ -3468,7 +3486,7 @@
         <v>19</v>
       </c>
       <c r="G69" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H69" t="b">
         <v>0</v>
@@ -3506,7 +3524,7 @@
         <v>23</v>
       </c>
       <c r="D70" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E70" t="s">
         <v>19</v>
@@ -3515,7 +3533,7 @@
         <v>19</v>
       </c>
       <c r="G70" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H70" t="b">
         <v>0</v>
@@ -3553,7 +3571,7 @@
         <v>23</v>
       </c>
       <c r="D71" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
@@ -3562,7 +3580,7 @@
         <v>19</v>
       </c>
       <c r="G71" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H71" t="b">
         <v>0</v>
@@ -3600,7 +3618,7 @@
         <v>23</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
@@ -3647,7 +3665,7 @@
         <v>23</v>
       </c>
       <c r="D73" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
@@ -3656,7 +3674,7 @@
         <v>19</v>
       </c>
       <c r="G73" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H73" t="b">
         <v>0</v>
@@ -3694,7 +3712,7 @@
         <v>23</v>
       </c>
       <c r="D74" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
@@ -3741,7 +3759,7 @@
         <v>23</v>
       </c>
       <c r="D75" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E75" t="s">
         <v>19</v>
@@ -3782,10 +3800,10 @@
         <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C77" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D77" t="s">
         <v>18</v>
@@ -3824,7 +3842,7 @@
         <v>21</v>
       </c>
       <c r="P77" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:16">
@@ -3838,7 +3856,7 @@
         <v>23</v>
       </c>
       <c r="D78" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
@@ -3885,7 +3903,7 @@
         <v>23</v>
       </c>
       <c r="D79" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
@@ -3932,7 +3950,7 @@
         <v>23</v>
       </c>
       <c r="D80" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
@@ -3979,7 +3997,7 @@
         <v>23</v>
       </c>
       <c r="D81" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
@@ -4026,7 +4044,7 @@
         <v>23</v>
       </c>
       <c r="D82" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
@@ -4035,7 +4053,7 @@
         <v>19</v>
       </c>
       <c r="G82" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H82" t="b">
         <v>0</v>
@@ -4073,7 +4091,7 @@
         <v>23</v>
       </c>
       <c r="D83" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
@@ -4082,7 +4100,7 @@
         <v>19</v>
       </c>
       <c r="G83" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H83" t="b">
         <v>0</v>
@@ -4120,7 +4138,7 @@
         <v>23</v>
       </c>
       <c r="D84" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
@@ -4129,7 +4147,7 @@
         <v>19</v>
       </c>
       <c r="G84" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H84" t="b">
         <v>0</v>
@@ -4167,7 +4185,7 @@
         <v>23</v>
       </c>
       <c r="D85" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E85" t="s">
         <v>19</v>
@@ -4214,7 +4232,7 @@
         <v>23</v>
       </c>
       <c r="D86" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
@@ -4261,7 +4279,7 @@
         <v>23</v>
       </c>
       <c r="D87" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
@@ -4308,7 +4326,7 @@
         <v>23</v>
       </c>
       <c r="D88" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
@@ -4349,10 +4367,10 @@
         <v>1</v>
       </c>
       <c r="B90" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C90" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D90" t="s">
         <v>18</v>
@@ -4391,7 +4409,7 @@
         <v>21</v>
       </c>
       <c r="P90" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:16">
@@ -4405,7 +4423,7 @@
         <v>23</v>
       </c>
       <c r="D91" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
@@ -4452,7 +4470,7 @@
         <v>23</v>
       </c>
       <c r="D92" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
@@ -4496,7 +4514,7 @@
         <v>27</v>
       </c>
       <c r="C94" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D94" t="s">
         <v>18</v>
@@ -4643,7 +4661,7 @@
         <v>23</v>
       </c>
       <c r="D97" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
@@ -4690,7 +4708,7 @@
         <v>23</v>
       </c>
       <c r="D98" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E98" t="s">
         <v>19</v>
@@ -4734,7 +4752,7 @@
         <v>16</v>
       </c>
       <c r="C100" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D100" t="s">
         <v>18</v>
@@ -4881,7 +4899,7 @@
         <v>23</v>
       </c>
       <c r="D103" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E103" t="s">
         <v>19</v>
@@ -4928,7 +4946,7 @@
         <v>23</v>
       </c>
       <c r="D104" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
@@ -4972,7 +4990,7 @@
         <v>37</v>
       </c>
       <c r="C106" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D106" t="s">
         <v>18</v>
@@ -5113,10 +5131,10 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C110" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D110" t="s">
         <v>18</v>
@@ -5155,7 +5173,7 @@
         <v>21</v>
       </c>
       <c r="P110" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="111" spans="1:16">
@@ -5169,7 +5187,7 @@
         <v>23</v>
       </c>
       <c r="D111" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E111" t="s">
         <v>19</v>
@@ -5216,7 +5234,7 @@
         <v>23</v>
       </c>
       <c r="D112" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E112" t="s">
         <v>19</v>
@@ -5257,10 +5275,10 @@
         <v>5</v>
       </c>
       <c r="B114" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C114" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D114" t="s">
         <v>18</v>
@@ -5299,7 +5317,7 @@
         <v>21</v>
       </c>
       <c r="P114" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="115" spans="1:16">
@@ -5313,7 +5331,7 @@
         <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E115" t="s">
         <v>19</v>
@@ -5322,7 +5340,7 @@
         <v>19</v>
       </c>
       <c r="G115" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H115" t="b">
         <v>0</v>
@@ -5360,7 +5378,7 @@
         <v>23</v>
       </c>
       <c r="D116" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E116" t="s">
         <v>19</v>
@@ -5407,7 +5425,7 @@
         <v>23</v>
       </c>
       <c r="D117" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E117" t="s">
         <v>19</v>
@@ -5454,7 +5472,7 @@
         <v>23</v>
       </c>
       <c r="D118" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E118" t="s">
         <v>19</v>
@@ -5495,10 +5513,10 @@
         <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C120" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D120" t="s">
         <v>18</v>
@@ -5537,7 +5555,7 @@
         <v>21</v>
       </c>
       <c r="P120" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:16">
@@ -5551,7 +5569,7 @@
         <v>23</v>
       </c>
       <c r="D121" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E121" t="s">
         <v>19</v>
@@ -5560,7 +5578,7 @@
         <v>19</v>
       </c>
       <c r="G121" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H121" t="b">
         <v>0</v>
@@ -5598,7 +5616,7 @@
         <v>23</v>
       </c>
       <c r="D122" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -5607,7 +5625,7 @@
         <v>19</v>
       </c>
       <c r="G122" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H122" t="b">
         <v>0</v>
@@ -5645,7 +5663,7 @@
         <v>23</v>
       </c>
       <c r="D123" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E123">
         <v>0</v>
@@ -5654,7 +5672,7 @@
         <v>19</v>
       </c>
       <c r="G123" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H123" t="b">
         <v>0</v>
@@ -5692,7 +5710,7 @@
         <v>23</v>
       </c>
       <c r="D124" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -5701,7 +5719,7 @@
         <v>19</v>
       </c>
       <c r="G124" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H124" t="b">
         <v>0</v>
@@ -5739,7 +5757,7 @@
         <v>23</v>
       </c>
       <c r="D125" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E125" t="s">
         <v>19</v>
@@ -5786,7 +5804,7 @@
         <v>23</v>
       </c>
       <c r="D126" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E126" t="s">
         <v>19</v>
@@ -5833,7 +5851,7 @@
         <v>23</v>
       </c>
       <c r="D127" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E127" t="s">
         <v>19</v>
@@ -5874,10 +5892,10 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C129" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D129" t="s">
         <v>18</v>
@@ -5916,7 +5934,7 @@
         <v>21</v>
       </c>
       <c r="P129" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="130" spans="1:16">
@@ -5930,7 +5948,7 @@
         <v>23</v>
       </c>
       <c r="D130" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E130" t="s">
         <v>19</v>
@@ -5977,7 +5995,7 @@
         <v>23</v>
       </c>
       <c r="D131" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E131" t="s">
         <v>19</v>
@@ -6018,10 +6036,10 @@
         <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C133" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D133" t="s">
         <v>18</v>
@@ -6060,7 +6078,7 @@
         <v>21</v>
       </c>
       <c r="P133" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="134" spans="1:16">
@@ -6074,7 +6092,7 @@
         <v>23</v>
       </c>
       <c r="D134" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E134" t="s">
         <v>19</v>
@@ -6121,7 +6139,7 @@
         <v>23</v>
       </c>
       <c r="D135" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E135" t="s">
         <v>19</v>
@@ -6168,7 +6186,7 @@
         <v>23</v>
       </c>
       <c r="D136" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E136">
         <v>0</v>
@@ -6177,7 +6195,7 @@
         <v>19</v>
       </c>
       <c r="G136" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H136" t="b">
         <v>0</v>
@@ -6215,7 +6233,7 @@
         <v>23</v>
       </c>
       <c r="D137" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E137" t="s">
         <v>19</v>
@@ -6262,7 +6280,7 @@
         <v>23</v>
       </c>
       <c r="D138" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E138" t="s">
         <v>19</v>
@@ -6309,7 +6327,7 @@
         <v>23</v>
       </c>
       <c r="D139" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E139" t="s">
         <v>19</v>
@@ -6350,10 +6368,10 @@
         <v>7</v>
       </c>
       <c r="B141" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C141" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D141" t="s">
         <v>18</v>
@@ -6392,7 +6410,7 @@
         <v>21</v>
       </c>
       <c r="P141" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="142" spans="1:16">
@@ -6406,7 +6424,7 @@
         <v>23</v>
       </c>
       <c r="D142" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -6415,7 +6433,7 @@
         <v>19</v>
       </c>
       <c r="G142" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="H142" t="b">
         <v>0</v>
@@ -6453,7 +6471,7 @@
         <v>23</v>
       </c>
       <c r="D143" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -6462,7 +6480,7 @@
         <v>19</v>
       </c>
       <c r="G143" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H143" t="b">
         <v>0</v>
@@ -6500,7 +6518,7 @@
         <v>23</v>
       </c>
       <c r="D144" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -6509,7 +6527,7 @@
         <v>19</v>
       </c>
       <c r="G144" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H144" t="b">
         <v>0</v>
@@ -6547,7 +6565,7 @@
         <v>23</v>
       </c>
       <c r="D145" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E145" t="s">
         <v>19</v>
@@ -6594,7 +6612,7 @@
         <v>23</v>
       </c>
       <c r="D146" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E146" t="s">
         <v>19</v>
@@ -6638,7 +6656,7 @@
         <v>37</v>
       </c>
       <c r="C148" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D148" t="s">
         <v>18</v>
@@ -6677,7 +6695,7 @@
         <v>21</v>
       </c>
       <c r="P148" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="149" spans="1:16">
@@ -6691,7 +6709,7 @@
         <v>23</v>
       </c>
       <c r="D149" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E149" t="s">
         <v>19</v>
@@ -6738,7 +6756,7 @@
         <v>23</v>
       </c>
       <c r="D150" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E150" t="s">
         <v>19</v>
@@ -6785,7 +6803,7 @@
         <v>23</v>
       </c>
       <c r="D151" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E151" t="s">
         <v>19</v>
@@ -6832,7 +6850,7 @@
         <v>23</v>
       </c>
       <c r="D152" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E152">
         <v>0</v>
@@ -6841,7 +6859,7 @@
         <v>19</v>
       </c>
       <c r="G152" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="H152" t="b">
         <v>0</v>
@@ -6879,7 +6897,7 @@
         <v>23</v>
       </c>
       <c r="D153" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E153">
         <v>0</v>
@@ -6888,7 +6906,7 @@
         <v>19</v>
       </c>
       <c r="G153" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="H153" t="b">
         <v>0</v>
@@ -6926,7 +6944,7 @@
         <v>23</v>
       </c>
       <c r="D154" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E154">
         <v>0</v>
@@ -6935,7 +6953,7 @@
         <v>19</v>
       </c>
       <c r="G154" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H154" t="b">
         <v>0</v>
@@ -6973,7 +6991,7 @@
         <v>23</v>
       </c>
       <c r="D155" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E155" t="s">
         <v>19</v>
@@ -7020,7 +7038,7 @@
         <v>23</v>
       </c>
       <c r="D156" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E156" t="s">
         <v>19</v>
@@ -7067,7 +7085,7 @@
         <v>23</v>
       </c>
       <c r="D157" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E157" t="s">
         <v>19</v>
@@ -7076,7 +7094,7 @@
         <v>19</v>
       </c>
       <c r="G157" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H157" t="b">
         <v>0</v>
@@ -7108,10 +7126,10 @@
         <v>1</v>
       </c>
       <c r="B159" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C159" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D159" t="s">
         <v>18</v>
@@ -7150,7 +7168,7 @@
         <v>21</v>
       </c>
       <c r="P159" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="160" spans="1:16">
@@ -7164,7 +7182,7 @@
         <v>23</v>
       </c>
       <c r="D160" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E160" t="s">
         <v>19</v>
@@ -7211,7 +7229,7 @@
         <v>23</v>
       </c>
       <c r="D161" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E161" t="s">
         <v>19</v>
@@ -7252,10 +7270,10 @@
         <v>5</v>
       </c>
       <c r="B163" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C163" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D163" t="s">
         <v>18</v>
@@ -7294,7 +7312,7 @@
         <v>21</v>
       </c>
       <c r="P163" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="164" spans="1:16">
@@ -7308,7 +7326,7 @@
         <v>23</v>
       </c>
       <c r="D164" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E164" t="s">
         <v>19</v>
@@ -7355,7 +7373,7 @@
         <v>23</v>
       </c>
       <c r="D165" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E165" t="s">
         <v>19</v>
@@ -7402,7 +7420,7 @@
         <v>23</v>
       </c>
       <c r="D166" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E166" t="s">
         <v>19</v>
@@ -7449,7 +7467,7 @@
         <v>23</v>
       </c>
       <c r="D167" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E167" t="s">
         <v>19</v>
@@ -7458,7 +7476,7 @@
         <v>19</v>
       </c>
       <c r="G167" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H167" t="b">
         <v>0</v>
@@ -7490,10 +7508,10 @@
         <v>5</v>
       </c>
       <c r="B169" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C169" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D169" t="s">
         <v>18</v>
@@ -7532,7 +7550,7 @@
         <v>21</v>
       </c>
       <c r="P169" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="170" spans="1:16">
@@ -7546,7 +7564,7 @@
         <v>23</v>
       </c>
       <c r="D170" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E170" t="s">
         <v>19</v>
@@ -7593,7 +7611,7 @@
         <v>23</v>
       </c>
       <c r="D171" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E171" t="s">
         <v>19</v>
@@ -7640,7 +7658,7 @@
         <v>23</v>
       </c>
       <c r="D172" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E172" t="s">
         <v>19</v>
@@ -7687,7 +7705,7 @@
         <v>23</v>
       </c>
       <c r="D173" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E173" t="s">
         <v>19</v>
@@ -7696,7 +7714,7 @@
         <v>19</v>
       </c>
       <c r="G173" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H173" t="b">
         <v>0</v>
@@ -7728,10 +7746,10 @@
         <v>6</v>
       </c>
       <c r="B175" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C175" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D175" t="s">
         <v>18</v>
@@ -7770,7 +7788,7 @@
         <v>21</v>
       </c>
       <c r="P175" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="176" spans="1:16">
@@ -7784,7 +7802,7 @@
         <v>23</v>
       </c>
       <c r="D176" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E176" t="s">
         <v>19</v>
@@ -7831,7 +7849,7 @@
         <v>23</v>
       </c>
       <c r="D177" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E177" t="s">
         <v>19</v>
@@ -7878,7 +7896,7 @@
         <v>23</v>
       </c>
       <c r="D178" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E178" t="s">
         <v>19</v>
@@ -7925,7 +7943,7 @@
         <v>23</v>
       </c>
       <c r="D179" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="E179" t="s">
         <v>19</v>
@@ -7934,7 +7952,7 @@
         <v>19</v>
       </c>
       <c r="G179" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H179" t="b">
         <v>0</v>
@@ -7966,10 +7984,10 @@
         <v>5</v>
       </c>
       <c r="B181" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C181" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D181" t="s">
         <v>18</v>
@@ -8008,7 +8026,7 @@
         <v>21</v>
       </c>
       <c r="P181" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="182" spans="1:16">
@@ -8022,7 +8040,7 @@
         <v>23</v>
       </c>
       <c r="D182" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E182" t="s">
         <v>19</v>
@@ -8069,7 +8087,7 @@
         <v>23</v>
       </c>
       <c r="D183" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E183" t="s">
         <v>19</v>
@@ -8116,7 +8134,7 @@
         <v>23</v>
       </c>
       <c r="D184" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E184" t="s">
         <v>19</v>
@@ -8125,7 +8143,7 @@
         <v>19</v>
       </c>
       <c r="G184" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H184" t="b">
         <v>0</v>
@@ -8157,10 +8175,10 @@
         <v>5</v>
       </c>
       <c r="B186" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C186" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D186" t="s">
         <v>18</v>
@@ -8199,7 +8217,7 @@
         <v>21</v>
       </c>
       <c r="P186" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="187" spans="1:16">
@@ -8213,7 +8231,7 @@
         <v>23</v>
       </c>
       <c r="D187" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E187" t="s">
         <v>19</v>
@@ -8260,7 +8278,7 @@
         <v>23</v>
       </c>
       <c r="D188" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E188" t="s">
         <v>19</v>
@@ -8307,7 +8325,7 @@
         <v>23</v>
       </c>
       <c r="D189" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E189" t="s">
         <v>19</v>
@@ -8316,7 +8334,7 @@
         <v>19</v>
       </c>
       <c r="G189" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H189" t="b">
         <v>0</v>
@@ -8348,10 +8366,10 @@
         <v>6</v>
       </c>
       <c r="B191" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C191" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D191" t="s">
         <v>18</v>
@@ -8390,7 +8408,7 @@
         <v>21</v>
       </c>
       <c r="P191" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="192" spans="1:16">
@@ -8404,7 +8422,7 @@
         <v>23</v>
       </c>
       <c r="D192" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E192" t="s">
         <v>19</v>
@@ -8413,7 +8431,7 @@
         <v>19</v>
       </c>
       <c r="G192" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H192" t="b">
         <v>0</v>
@@ -8451,7 +8469,7 @@
         <v>23</v>
       </c>
       <c r="D193" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E193" t="s">
         <v>19</v>
@@ -8498,7 +8516,7 @@
         <v>23</v>
       </c>
       <c r="D194" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E194" t="s">
         <v>19</v>
@@ -8539,10 +8557,10 @@
         <v>7</v>
       </c>
       <c r="B196" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C196" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D196" t="s">
         <v>18</v>
@@ -8581,7 +8599,7 @@
         <v>21</v>
       </c>
       <c r="P196" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="197" spans="1:16">
@@ -8595,7 +8613,7 @@
         <v>23</v>
       </c>
       <c r="D197" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E197">
         <v>0</v>
@@ -8604,7 +8622,7 @@
         <v>19</v>
       </c>
       <c r="G197" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="H197" t="b">
         <v>0</v>
@@ -8642,7 +8660,7 @@
         <v>23</v>
       </c>
       <c r="D198" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E198" t="s">
         <v>19</v>
@@ -8651,7 +8669,7 @@
         <v>19</v>
       </c>
       <c r="G198" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H198" t="b">
         <v>0</v>
@@ -8689,7 +8707,7 @@
         <v>23</v>
       </c>
       <c r="D199" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E199" t="s">
         <v>19</v>
@@ -8736,7 +8754,7 @@
         <v>23</v>
       </c>
       <c r="D200" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E200" t="s">
         <v>19</v>
@@ -8783,7 +8801,7 @@
         <v>23</v>
       </c>
       <c r="D201" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E201" t="s">
         <v>19</v>
@@ -8830,7 +8848,7 @@
         <v>23</v>
       </c>
       <c r="D202" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E202" t="s">
         <v>19</v>
@@ -8877,7 +8895,7 @@
         <v>23</v>
       </c>
       <c r="D203" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E203" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updated Tables / Data Dict
- Description fields can now be null
- Addresses now default to United States Houston Texas 77339 4534 YourStreet Name
- Phone numbers now have a validator on the gui
</commit_message>
<xml_diff>
--- a/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
+++ b/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="183">
   <si>
     <t>Load Order</t>
   </si>
@@ -82,7 +82,7 @@
     <t>Standard Auto-Increment PK</t>
   </si>
   <si>
-    <t>Allows for multiple named labels</t>
+    <t>Categorizes customers based on the opinion of the store owner.</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -103,6 +103,9 @@
     <t>EmployeeCategory</t>
   </si>
   <si>
+    <t>Categorizes employee based on the opinion of the store owner.</t>
+  </si>
+  <si>
     <t>Alanna Gilcrease</t>
   </si>
   <si>
@@ -184,7 +187,7 @@
     <t>StateProvince</t>
   </si>
   <si>
-    <t>Blank Description</t>
+    <t>The state/province that a particular entity (a store, a customer) is located in.</t>
   </si>
   <si>
     <t>state_name</t>
@@ -205,12 +208,21 @@
     <t>zip_code</t>
   </si>
   <si>
+    <t>77339</t>
+  </si>
+  <si>
     <t>city</t>
   </si>
   <si>
+    <t>Houston</t>
+  </si>
+  <si>
     <t>address</t>
   </si>
   <si>
+    <t>3242 StreetName</t>
+  </si>
+  <si>
     <t>state_id</t>
   </si>
   <si>
@@ -223,9 +235,15 @@
     <t>EmployeeType</t>
   </si>
   <si>
+    <t xml:space="preserve">The working type of an employee such as part-time or full-time. </t>
+  </si>
+  <si>
     <t>Employee</t>
   </si>
   <si>
+    <t>Person that works at the store and deals with either the store products or maintenance of said store.</t>
+  </si>
+  <si>
     <t>first_name</t>
   </si>
   <si>
@@ -238,6 +256,9 @@
     <t>phone_number</t>
   </si>
   <si>
+    <t>PhoneNumberField</t>
+  </si>
+  <si>
     <t>comments</t>
   </si>
   <si>
@@ -271,6 +292,9 @@
     <t>Customer</t>
   </si>
   <si>
+    <t>Someone who potentially purchases an item/service from our client and whose general information has been collected by our loyalty system database.</t>
+  </si>
+  <si>
     <t>create_employee_id</t>
   </si>
   <si>
@@ -283,6 +307,9 @@
     <t>Job</t>
   </si>
   <si>
+    <t>The type of role that an employee of a store holds such as cashier, manager, etc.</t>
+  </si>
+  <si>
     <t>job_name</t>
   </si>
   <si>
@@ -292,6 +319,9 @@
     <t>EmployeeEmployeeCategory</t>
   </si>
   <si>
+    <t>Allows an employee to have multiple categories</t>
+  </si>
+  <si>
     <t>employee_id</t>
   </si>
   <si>
@@ -301,6 +331,9 @@
     <t>CustomerCustomerCategory</t>
   </si>
   <si>
+    <t>Allows a customer to have multiple categories</t>
+  </si>
+  <si>
     <t>customer_id</t>
   </si>
   <si>
@@ -310,15 +343,24 @@
     <t>PaymentType</t>
   </si>
   <si>
+    <t>The way a customer pays for a service or product such as cash, credit, Google Pay, etc.</t>
+  </si>
+  <si>
     <t>Store</t>
   </si>
   <si>
+    <t>A physical location where customers go to complete transactions.</t>
+  </si>
+  <si>
     <t>store_status_id</t>
   </si>
   <si>
     <t>EmployeeJob</t>
   </si>
   <si>
+    <t>Allows an employee to have multiple jobs at the same or different stores.</t>
+  </si>
+  <si>
     <t>assign_date</t>
   </si>
   <si>
@@ -334,6 +376,9 @@
     <t>Order</t>
   </si>
   <si>
+    <t>The customer’s finalized transaction of products purchased. This order generates customer loyalty points based on the monetary total of the transaction.</t>
+  </si>
+  <si>
     <t>order_date</t>
   </si>
   <si>
@@ -355,6 +400,9 @@
     <t>ProductType</t>
   </si>
   <si>
+    <t xml:space="preserve"> Identifying certain product types that are eligible to be purchased with points, versus products that are not eligible to earn points on; used to distinguish exclusions. </t>
+  </si>
+  <si>
     <t>product_type_name</t>
   </si>
   <si>
@@ -364,6 +412,9 @@
     <t>Product</t>
   </si>
   <si>
+    <t>An item purchased by the customer in a transaction.</t>
+  </si>
+  <si>
     <t>product_name</t>
   </si>
   <si>
@@ -385,6 +436,9 @@
     <t>OrderLine</t>
   </si>
   <si>
+    <t>Represents information located on a singular line found on a receipt/invoice produced after a completed transaction that describes the customer’s transaction and product details (quantity, product type, total price for that order line).</t>
+  </si>
+  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -433,6 +487,9 @@
     <t>SocialMediaType</t>
   </si>
   <si>
+    <t>The different types of social media that exist for use such as Instagram, Snapchat, etc.</t>
+  </si>
+  <si>
     <t>social_media_name</t>
   </si>
   <si>
@@ -445,6 +502,9 @@
     <t>StoreSocialMedia</t>
   </si>
   <si>
+    <t>Social media of the store.</t>
+  </si>
+  <si>
     <t>social_media_code</t>
   </si>
   <si>
@@ -454,18 +514,30 @@
     <t>EmployeeSocialMedia</t>
   </si>
   <si>
+    <t>Employee social media.</t>
+  </si>
+  <si>
     <t>CustomerSocialMedia</t>
   </si>
   <si>
+    <t>Customer social media.</t>
+  </si>
+  <si>
     <t>StoreProduct</t>
   </si>
   <si>
+    <t>Products that are either associated with or are offered at a specific store location.</t>
+  </si>
+  <si>
     <t>product_assigned</t>
   </si>
   <si>
     <t>Store Reward</t>
   </si>
   <si>
+    <t>Rewards available to loyalty customers based on which specific store points are redeemed at.</t>
+  </si>
+  <si>
     <t>reward_id</t>
   </si>
   <si>
@@ -475,10 +547,16 @@
     <t>CustomerReward</t>
   </si>
   <si>
+    <t>Rewards available to a SINGLE loyalty customer to be redeemed, based on the amount of points they have accumulated to date. Available rewards that they (a single loyalty customer) has earned, based on their personal points. A points bank.</t>
+  </si>
+  <si>
     <t>date_applied</t>
   </si>
   <si>
     <t>PointLog</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Keeping track of a customers existing loyalty points and used points?</t>
   </si>
   <si>
     <t>reason_id</t>
@@ -851,9 +929,9 @@
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
@@ -1041,10 +1119,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="b">
         <v>0</v>
@@ -1106,7 +1184,7 @@
         <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1185,10 +1263,10 @@
         <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" t="b">
         <v>0</v>
@@ -1208,10 +1286,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -1250,7 +1328,7 @@
         <v>21</v>
       </c>
       <c r="P10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1264,7 +1342,7 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
@@ -1311,7 +1389,7 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
@@ -1329,10 +1407,10 @@
         <v>0</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" t="b">
         <v>0</v>
@@ -1358,7 +1436,7 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -1367,7 +1445,7 @@
         <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1391,7 +1469,7 @@
         <v>19</v>
       </c>
       <c r="O13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P13" t="s">
         <v>23</v>
@@ -1402,10 +1480,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
@@ -1444,7 +1522,7 @@
         <v>21</v>
       </c>
       <c r="P15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1458,7 +1536,7 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
@@ -1505,7 +1583,7 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -1523,10 +1601,10 @@
         <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="b">
         <v>0</v>
@@ -1552,7 +1630,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
@@ -1561,7 +1639,7 @@
         <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -1585,7 +1663,7 @@
         <v>19</v>
       </c>
       <c r="O18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P18" t="s">
         <v>23</v>
@@ -1596,10 +1674,10 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
@@ -1638,7 +1716,7 @@
         <v>21</v>
       </c>
       <c r="P20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1652,7 +1730,7 @@
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -1699,7 +1777,7 @@
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
@@ -1717,10 +1795,10 @@
         <v>0</v>
       </c>
       <c r="J22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" t="b">
         <v>0</v>
@@ -1746,7 +1824,7 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -1755,7 +1833,7 @@
         <v>19</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -1779,7 +1857,7 @@
         <v>19</v>
       </c>
       <c r="O23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P23" t="s">
         <v>23</v>
@@ -1790,10 +1868,10 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -1832,7 +1910,7 @@
         <v>21</v>
       </c>
       <c r="P25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1846,7 +1924,7 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -1893,7 +1971,7 @@
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
@@ -1911,10 +1989,10 @@
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" t="b">
         <v>0</v>
@@ -1940,7 +2018,7 @@
         <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -1949,7 +2027,7 @@
         <v>19</v>
       </c>
       <c r="G28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
@@ -1973,7 +2051,7 @@
         <v>19</v>
       </c>
       <c r="O28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P28" t="s">
         <v>23</v>
@@ -1984,10 +2062,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
         <v>18</v>
@@ -2026,7 +2104,7 @@
         <v>21</v>
       </c>
       <c r="P30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2040,7 +2118,7 @@
         <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
@@ -2087,7 +2165,7 @@
         <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
@@ -2105,10 +2183,10 @@
         <v>0</v>
       </c>
       <c r="J32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32" t="b">
         <v>0</v>
@@ -2134,7 +2212,7 @@
         <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
@@ -2143,7 +2221,7 @@
         <v>19</v>
       </c>
       <c r="G33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -2167,7 +2245,7 @@
         <v>19</v>
       </c>
       <c r="O33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P33" t="s">
         <v>23</v>
@@ -2178,10 +2256,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
@@ -2220,7 +2298,7 @@
         <v>21</v>
       </c>
       <c r="P35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2299,10 +2377,10 @@
         <v>0</v>
       </c>
       <c r="J37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" t="b">
         <v>0</v>
@@ -2322,10 +2400,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D39" t="s">
         <v>18</v>
@@ -2364,7 +2442,7 @@
         <v>21</v>
       </c>
       <c r="P39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -2443,10 +2521,10 @@
         <v>0</v>
       </c>
       <c r="J41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" t="b">
         <v>0</v>
@@ -2469,7 +2547,7 @@
         <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D43" t="s">
         <v>18</v>
@@ -2508,7 +2586,7 @@
         <v>21</v>
       </c>
       <c r="P43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -2522,7 +2600,7 @@
         <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
@@ -2566,7 +2644,7 @@
         <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
@@ -2605,7 +2683,7 @@
         <v>21</v>
       </c>
       <c r="P46" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -2619,7 +2697,7 @@
         <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
@@ -2666,10 +2744,10 @@
         <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
-      </c>
-      <c r="E48" t="s">
-        <v>19</v>
+        <v>59</v>
+      </c>
+      <c r="E48">
+        <v>233</v>
       </c>
       <c r="F48" t="s">
         <v>19</v>
@@ -2707,10 +2785,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
         <v>18</v>
@@ -2749,7 +2827,7 @@
         <v>21</v>
       </c>
       <c r="P50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -2763,10 +2841,10 @@
         <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E51" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="F51">
         <v>10</v>
@@ -2810,10 +2888,10 @@
         <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="F52">
         <v>35</v>
@@ -2857,10 +2935,10 @@
         <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E53" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="F53">
         <v>100</v>
@@ -2904,10 +2982,10 @@
         <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>65</v>
-      </c>
-      <c r="E54" t="s">
-        <v>19</v>
+        <v>69</v>
+      </c>
+      <c r="E54">
+        <v>1407</v>
       </c>
       <c r="F54" t="s">
         <v>19</v>
@@ -2945,10 +3023,10 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D56" t="s">
         <v>18</v>
@@ -2987,7 +3065,7 @@
         <v>21</v>
       </c>
       <c r="P56" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -3066,10 +3144,10 @@
         <v>0</v>
       </c>
       <c r="J58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58" t="b">
         <v>0</v>
@@ -3092,7 +3170,7 @@
         <v>27</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
@@ -3131,7 +3209,7 @@
         <v>21</v>
       </c>
       <c r="P60" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -3210,10 +3288,10 @@
         <v>0</v>
       </c>
       <c r="J62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L62" t="b">
         <v>0</v>
@@ -3233,10 +3311,10 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D64" t="s">
         <v>18</v>
@@ -3275,7 +3353,7 @@
         <v>21</v>
       </c>
       <c r="P64" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -3289,7 +3367,7 @@
         <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E65" t="s">
         <v>19</v>
@@ -3336,7 +3414,7 @@
         <v>23</v>
       </c>
       <c r="D66" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E66" t="s">
         <v>19</v>
@@ -3383,7 +3461,7 @@
         <v>23</v>
       </c>
       <c r="D67" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E67" t="s">
         <v>19</v>
@@ -3430,16 +3508,16 @@
         <v>23</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E68" t="s">
         <v>19</v>
       </c>
       <c r="F68">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G68" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="H68" t="b">
         <v>0</v>
@@ -3477,13 +3555,13 @@
         <v>23</v>
       </c>
       <c r="D69" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
       </c>
       <c r="F69" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G69" t="s">
         <v>25</v>
@@ -3524,7 +3602,7 @@
         <v>23</v>
       </c>
       <c r="D70" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E70" t="s">
         <v>19</v>
@@ -3533,7 +3611,7 @@
         <v>19</v>
       </c>
       <c r="G70" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H70" t="b">
         <v>0</v>
@@ -3571,7 +3649,7 @@
         <v>23</v>
       </c>
       <c r="D71" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
@@ -3580,7 +3658,7 @@
         <v>19</v>
       </c>
       <c r="G71" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H71" t="b">
         <v>0</v>
@@ -3618,7 +3696,7 @@
         <v>23</v>
       </c>
       <c r="D72" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
@@ -3665,7 +3743,7 @@
         <v>23</v>
       </c>
       <c r="D73" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
@@ -3674,7 +3752,7 @@
         <v>19</v>
       </c>
       <c r="G73" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H73" t="b">
         <v>0</v>
@@ -3712,7 +3790,7 @@
         <v>23</v>
       </c>
       <c r="D74" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E74" t="s">
         <v>19</v>
@@ -3759,7 +3837,7 @@
         <v>23</v>
       </c>
       <c r="D75" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E75" t="s">
         <v>19</v>
@@ -3800,10 +3878,10 @@
         <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C77" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D77" t="s">
         <v>18</v>
@@ -3842,7 +3920,7 @@
         <v>21</v>
       </c>
       <c r="P77" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:16">
@@ -3856,7 +3934,7 @@
         <v>23</v>
       </c>
       <c r="D78" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E78" t="s">
         <v>19</v>
@@ -3903,7 +3981,7 @@
         <v>23</v>
       </c>
       <c r="D79" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E79" t="s">
         <v>19</v>
@@ -3950,7 +4028,7 @@
         <v>23</v>
       </c>
       <c r="D80" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E80" t="s">
         <v>19</v>
@@ -3997,16 +4075,16 @@
         <v>23</v>
       </c>
       <c r="D81" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E81" t="s">
         <v>19</v>
       </c>
       <c r="F81">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G81" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="H81" t="b">
         <v>0</v>
@@ -4044,13 +4122,13 @@
         <v>23</v>
       </c>
       <c r="D82" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
       </c>
       <c r="F82" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G82" t="s">
         <v>25</v>
@@ -4091,7 +4169,7 @@
         <v>23</v>
       </c>
       <c r="D83" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E83" t="s">
         <v>19</v>
@@ -4100,7 +4178,7 @@
         <v>19</v>
       </c>
       <c r="G83" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H83" t="b">
         <v>0</v>
@@ -4138,7 +4216,7 @@
         <v>23</v>
       </c>
       <c r="D84" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E84" t="s">
         <v>19</v>
@@ -4147,7 +4225,7 @@
         <v>19</v>
       </c>
       <c r="G84" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H84" t="b">
         <v>0</v>
@@ -4185,7 +4263,7 @@
         <v>23</v>
       </c>
       <c r="D85" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E85" t="s">
         <v>19</v>
@@ -4232,7 +4310,7 @@
         <v>23</v>
       </c>
       <c r="D86" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E86" t="s">
         <v>19</v>
@@ -4279,7 +4357,7 @@
         <v>23</v>
       </c>
       <c r="D87" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E87" t="s">
         <v>19</v>
@@ -4326,7 +4404,7 @@
         <v>23</v>
       </c>
       <c r="D88" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E88" t="s">
         <v>19</v>
@@ -4367,10 +4445,10 @@
         <v>1</v>
       </c>
       <c r="B90" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C90" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D90" t="s">
         <v>18</v>
@@ -4409,7 +4487,7 @@
         <v>21</v>
       </c>
       <c r="P90" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:16">
@@ -4423,7 +4501,7 @@
         <v>23</v>
       </c>
       <c r="D91" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
@@ -4470,7 +4548,7 @@
         <v>23</v>
       </c>
       <c r="D92" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
@@ -4514,7 +4592,7 @@
         <v>27</v>
       </c>
       <c r="C94" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D94" t="s">
         <v>18</v>
@@ -4553,7 +4631,7 @@
         <v>21</v>
       </c>
       <c r="P94" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -4632,10 +4710,10 @@
         <v>0</v>
       </c>
       <c r="J96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L96" t="b">
         <v>0</v>
@@ -4661,7 +4739,7 @@
         <v>23</v>
       </c>
       <c r="D97" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E97" t="s">
         <v>19</v>
@@ -4708,7 +4786,7 @@
         <v>23</v>
       </c>
       <c r="D98" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E98" t="s">
         <v>19</v>
@@ -4752,7 +4830,7 @@
         <v>16</v>
       </c>
       <c r="C100" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D100" t="s">
         <v>18</v>
@@ -4791,7 +4869,7 @@
         <v>21</v>
       </c>
       <c r="P100" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:16">
@@ -4870,10 +4948,10 @@
         <v>0</v>
       </c>
       <c r="J102" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K102" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L102" t="b">
         <v>0</v>
@@ -4899,7 +4977,7 @@
         <v>23</v>
       </c>
       <c r="D103" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E103" t="s">
         <v>19</v>
@@ -4946,7 +5024,7 @@
         <v>23</v>
       </c>
       <c r="D104" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
@@ -4987,10 +5065,10 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C106" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="D106" t="s">
         <v>18</v>
@@ -5029,7 +5107,7 @@
         <v>21</v>
       </c>
       <c r="P106" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
     </row>
     <row r="107" spans="1:16">
@@ -5108,10 +5186,10 @@
         <v>0</v>
       </c>
       <c r="J108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K108" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L108" t="b">
         <v>0</v>
@@ -5131,10 +5209,10 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C110" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D110" t="s">
         <v>18</v>
@@ -5173,7 +5251,7 @@
         <v>21</v>
       </c>
       <c r="P110" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
     </row>
     <row r="111" spans="1:16">
@@ -5187,7 +5265,7 @@
         <v>23</v>
       </c>
       <c r="D111" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E111" t="s">
         <v>19</v>
@@ -5234,7 +5312,7 @@
         <v>23</v>
       </c>
       <c r="D112" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="E112" t="s">
         <v>19</v>
@@ -5275,10 +5353,10 @@
         <v>5</v>
       </c>
       <c r="B114" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C114" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D114" t="s">
         <v>18</v>
@@ -5317,7 +5395,7 @@
         <v>21</v>
       </c>
       <c r="P114" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:16">
@@ -5331,7 +5409,7 @@
         <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="E115" t="s">
         <v>19</v>
@@ -5340,7 +5418,7 @@
         <v>19</v>
       </c>
       <c r="G115" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H115" t="b">
         <v>0</v>
@@ -5378,7 +5456,7 @@
         <v>23</v>
       </c>
       <c r="D116" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E116" t="s">
         <v>19</v>
@@ -5425,7 +5503,7 @@
         <v>23</v>
       </c>
       <c r="D117" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E117" t="s">
         <v>19</v>
@@ -5472,7 +5550,7 @@
         <v>23</v>
       </c>
       <c r="D118" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="E118" t="s">
         <v>19</v>
@@ -5513,10 +5591,10 @@
         <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="D120" t="s">
         <v>18</v>
@@ -5555,7 +5633,7 @@
         <v>21</v>
       </c>
       <c r="P120" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:16">
@@ -5569,7 +5647,7 @@
         <v>23</v>
       </c>
       <c r="D121" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="E121" t="s">
         <v>19</v>
@@ -5578,7 +5656,7 @@
         <v>19</v>
       </c>
       <c r="G121" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H121" t="b">
         <v>0</v>
@@ -5616,7 +5694,7 @@
         <v>23</v>
       </c>
       <c r="D122" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -5625,7 +5703,7 @@
         <v>19</v>
       </c>
       <c r="G122" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="H122" t="b">
         <v>0</v>
@@ -5663,7 +5741,7 @@
         <v>23</v>
       </c>
       <c r="D123" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="E123">
         <v>0</v>
@@ -5672,7 +5750,7 @@
         <v>19</v>
       </c>
       <c r="G123" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="H123" t="b">
         <v>0</v>
@@ -5710,7 +5788,7 @@
         <v>23</v>
       </c>
       <c r="D124" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -5719,7 +5797,7 @@
         <v>19</v>
       </c>
       <c r="G124" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="H124" t="b">
         <v>0</v>
@@ -5757,7 +5835,7 @@
         <v>23</v>
       </c>
       <c r="D125" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E125" t="s">
         <v>19</v>
@@ -5804,7 +5882,7 @@
         <v>23</v>
       </c>
       <c r="D126" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="E126" t="s">
         <v>19</v>
@@ -5851,7 +5929,7 @@
         <v>23</v>
       </c>
       <c r="D127" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E127" t="s">
         <v>19</v>
@@ -5892,10 +5970,10 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C129" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="D129" t="s">
         <v>18</v>
@@ -5934,7 +6012,7 @@
         <v>21</v>
       </c>
       <c r="P129" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:16">
@@ -5948,7 +6026,7 @@
         <v>23</v>
       </c>
       <c r="D130" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="E130" t="s">
         <v>19</v>
@@ -5995,7 +6073,7 @@
         <v>23</v>
       </c>
       <c r="D131" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="E131" t="s">
         <v>19</v>
@@ -6013,10 +6091,10 @@
         <v>0</v>
       </c>
       <c r="J131" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K131" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L131" t="b">
         <v>0</v>
@@ -6036,10 +6114,10 @@
         <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C133" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="D133" t="s">
         <v>18</v>
@@ -6078,7 +6156,7 @@
         <v>21</v>
       </c>
       <c r="P133" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:16">
@@ -6092,7 +6170,7 @@
         <v>23</v>
       </c>
       <c r="D134" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="E134" t="s">
         <v>19</v>
@@ -6139,7 +6217,7 @@
         <v>23</v>
       </c>
       <c r="D135" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="E135" t="s">
         <v>19</v>
@@ -6157,10 +6235,10 @@
         <v>0</v>
       </c>
       <c r="J135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K135" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L135" t="b">
         <v>0</v>
@@ -6186,7 +6264,7 @@
         <v>23</v>
       </c>
       <c r="D136" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="E136">
         <v>0</v>
@@ -6195,7 +6273,7 @@
         <v>19</v>
       </c>
       <c r="G136" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="H136" t="b">
         <v>0</v>
@@ -6233,7 +6311,7 @@
         <v>23</v>
       </c>
       <c r="D137" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="E137" t="s">
         <v>19</v>
@@ -6280,7 +6358,7 @@
         <v>23</v>
       </c>
       <c r="D138" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="E138" t="s">
         <v>19</v>
@@ -6327,7 +6405,7 @@
         <v>23</v>
       </c>
       <c r="D139" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="E139" t="s">
         <v>19</v>
@@ -6368,10 +6446,10 @@
         <v>7</v>
       </c>
       <c r="B141" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C141" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="D141" t="s">
         <v>18</v>
@@ -6410,7 +6488,7 @@
         <v>21</v>
       </c>
       <c r="P141" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:16">
@@ -6424,7 +6502,7 @@
         <v>23</v>
       </c>
       <c r="D142" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -6433,7 +6511,7 @@
         <v>19</v>
       </c>
       <c r="G142" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="H142" t="b">
         <v>0</v>
@@ -6471,7 +6549,7 @@
         <v>23</v>
       </c>
       <c r="D143" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -6480,7 +6558,7 @@
         <v>19</v>
       </c>
       <c r="G143" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="H143" t="b">
         <v>0</v>
@@ -6518,7 +6596,7 @@
         <v>23</v>
       </c>
       <c r="D144" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -6527,7 +6605,7 @@
         <v>19</v>
       </c>
       <c r="G144" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="H144" t="b">
         <v>0</v>
@@ -6565,7 +6643,7 @@
         <v>23</v>
       </c>
       <c r="D145" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="E145" t="s">
         <v>19</v>
@@ -6612,7 +6690,7 @@
         <v>23</v>
       </c>
       <c r="D146" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="E146" t="s">
         <v>19</v>
@@ -6653,10 +6731,10 @@
         <v>3</v>
       </c>
       <c r="B148" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C148" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="D148" t="s">
         <v>18</v>
@@ -6695,7 +6773,7 @@
         <v>21</v>
       </c>
       <c r="P148" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="149" spans="1:16">
@@ -6709,7 +6787,7 @@
         <v>23</v>
       </c>
       <c r="D149" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="E149" t="s">
         <v>19</v>
@@ -6756,7 +6834,7 @@
         <v>23</v>
       </c>
       <c r="D150" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="E150" t="s">
         <v>19</v>
@@ -6774,10 +6852,10 @@
         <v>0</v>
       </c>
       <c r="J150" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K150" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L150" t="b">
         <v>0</v>
@@ -6803,7 +6881,7 @@
         <v>23</v>
       </c>
       <c r="D151" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="E151" t="s">
         <v>19</v>
@@ -6850,7 +6928,7 @@
         <v>23</v>
       </c>
       <c r="D152" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="E152">
         <v>0</v>
@@ -6859,7 +6937,7 @@
         <v>19</v>
       </c>
       <c r="G152" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="H152" t="b">
         <v>0</v>
@@ -6897,7 +6975,7 @@
         <v>23</v>
       </c>
       <c r="D153" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="E153">
         <v>0</v>
@@ -6906,7 +6984,7 @@
         <v>19</v>
       </c>
       <c r="G153" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="H153" t="b">
         <v>0</v>
@@ -6944,7 +7022,7 @@
         <v>23</v>
       </c>
       <c r="D154" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="E154">
         <v>0</v>
@@ -6953,7 +7031,7 @@
         <v>19</v>
       </c>
       <c r="G154" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="H154" t="b">
         <v>0</v>
@@ -6991,7 +7069,7 @@
         <v>23</v>
       </c>
       <c r="D155" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="E155" t="s">
         <v>19</v>
@@ -7038,7 +7116,7 @@
         <v>23</v>
       </c>
       <c r="D156" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E156" t="s">
         <v>19</v>
@@ -7085,7 +7163,7 @@
         <v>23</v>
       </c>
       <c r="D157" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="E157" t="s">
         <v>19</v>
@@ -7094,7 +7172,7 @@
         <v>19</v>
       </c>
       <c r="G157" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H157" t="b">
         <v>0</v>
@@ -7126,10 +7204,10 @@
         <v>1</v>
       </c>
       <c r="B159" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C159" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="D159" t="s">
         <v>18</v>
@@ -7168,7 +7246,7 @@
         <v>21</v>
       </c>
       <c r="P159" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:16">
@@ -7182,7 +7260,7 @@
         <v>23</v>
       </c>
       <c r="D160" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="E160" t="s">
         <v>19</v>
@@ -7229,7 +7307,7 @@
         <v>23</v>
       </c>
       <c r="D161" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E161" t="s">
         <v>19</v>
@@ -7247,10 +7325,10 @@
         <v>0</v>
       </c>
       <c r="J161" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K161" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L161" t="b">
         <v>0</v>
@@ -7270,10 +7348,10 @@
         <v>5</v>
       </c>
       <c r="B163" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="C163" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="D163" t="s">
         <v>18</v>
@@ -7312,7 +7390,7 @@
         <v>21</v>
       </c>
       <c r="P163" t="s">
-        <v>56</v>
+        <v>162</v>
       </c>
     </row>
     <row r="164" spans="1:16">
@@ -7326,7 +7404,7 @@
         <v>23</v>
       </c>
       <c r="D164" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E164" t="s">
         <v>19</v>
@@ -7373,7 +7451,7 @@
         <v>23</v>
       </c>
       <c r="D165" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E165" t="s">
         <v>19</v>
@@ -7420,7 +7498,7 @@
         <v>23</v>
       </c>
       <c r="D166" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="E166" t="s">
         <v>19</v>
@@ -7467,7 +7545,7 @@
         <v>23</v>
       </c>
       <c r="D167" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="E167" t="s">
         <v>19</v>
@@ -7476,7 +7554,7 @@
         <v>19</v>
       </c>
       <c r="G167" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H167" t="b">
         <v>0</v>
@@ -7508,10 +7586,10 @@
         <v>5</v>
       </c>
       <c r="B169" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="C169" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="D169" t="s">
         <v>18</v>
@@ -7550,7 +7628,7 @@
         <v>21</v>
       </c>
       <c r="P169" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
     </row>
     <row r="170" spans="1:16">
@@ -7564,7 +7642,7 @@
         <v>23</v>
       </c>
       <c r="D170" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E170" t="s">
         <v>19</v>
@@ -7611,7 +7689,7 @@
         <v>23</v>
       </c>
       <c r="D171" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E171" t="s">
         <v>19</v>
@@ -7658,7 +7736,7 @@
         <v>23</v>
       </c>
       <c r="D172" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="E172" t="s">
         <v>19</v>
@@ -7705,7 +7783,7 @@
         <v>23</v>
       </c>
       <c r="D173" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="E173" t="s">
         <v>19</v>
@@ -7714,7 +7792,7 @@
         <v>19</v>
       </c>
       <c r="G173" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H173" t="b">
         <v>0</v>
@@ -7746,10 +7824,10 @@
         <v>6</v>
       </c>
       <c r="B175" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C175" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="D175" t="s">
         <v>18</v>
@@ -7788,7 +7866,7 @@
         <v>21</v>
       </c>
       <c r="P175" t="s">
-        <v>56</v>
+        <v>168</v>
       </c>
     </row>
     <row r="176" spans="1:16">
@@ -7802,7 +7880,7 @@
         <v>23</v>
       </c>
       <c r="D176" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E176" t="s">
         <v>19</v>
@@ -7849,7 +7927,7 @@
         <v>23</v>
       </c>
       <c r="D177" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="E177" t="s">
         <v>19</v>
@@ -7896,7 +7974,7 @@
         <v>23</v>
       </c>
       <c r="D178" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E178" t="s">
         <v>19</v>
@@ -7943,7 +8021,7 @@
         <v>23</v>
       </c>
       <c r="D179" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="E179" t="s">
         <v>19</v>
@@ -7952,7 +8030,7 @@
         <v>19</v>
       </c>
       <c r="G179" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H179" t="b">
         <v>0</v>
@@ -7984,10 +8062,10 @@
         <v>5</v>
       </c>
       <c r="B181" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C181" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="D181" t="s">
         <v>18</v>
@@ -8026,7 +8104,7 @@
         <v>21</v>
       </c>
       <c r="P181" t="s">
-        <v>56</v>
+        <v>170</v>
       </c>
     </row>
     <row r="182" spans="1:16">
@@ -8040,7 +8118,7 @@
         <v>23</v>
       </c>
       <c r="D182" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="E182" t="s">
         <v>19</v>
@@ -8087,7 +8165,7 @@
         <v>23</v>
       </c>
       <c r="D183" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E183" t="s">
         <v>19</v>
@@ -8134,7 +8212,7 @@
         <v>23</v>
       </c>
       <c r="D184" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="E184" t="s">
         <v>19</v>
@@ -8143,7 +8221,7 @@
         <v>19</v>
       </c>
       <c r="G184" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H184" t="b">
         <v>0</v>
@@ -8175,10 +8253,10 @@
         <v>5</v>
       </c>
       <c r="B186" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="C186" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="D186" t="s">
         <v>18</v>
@@ -8217,7 +8295,7 @@
         <v>21</v>
       </c>
       <c r="P186" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
     </row>
     <row r="187" spans="1:16">
@@ -8231,7 +8309,7 @@
         <v>23</v>
       </c>
       <c r="D187" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="E187" t="s">
         <v>19</v>
@@ -8278,7 +8356,7 @@
         <v>23</v>
       </c>
       <c r="D188" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E188" t="s">
         <v>19</v>
@@ -8325,7 +8403,7 @@
         <v>23</v>
       </c>
       <c r="D189" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="E189" t="s">
         <v>19</v>
@@ -8334,7 +8412,7 @@
         <v>19</v>
       </c>
       <c r="G189" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H189" t="b">
         <v>0</v>
@@ -8366,10 +8444,10 @@
         <v>6</v>
       </c>
       <c r="B191" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C191" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="D191" t="s">
         <v>18</v>
@@ -8408,7 +8486,7 @@
         <v>21</v>
       </c>
       <c r="P191" t="s">
-        <v>56</v>
+        <v>177</v>
       </c>
     </row>
     <row r="192" spans="1:16">
@@ -8422,7 +8500,7 @@
         <v>23</v>
       </c>
       <c r="D192" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="E192" t="s">
         <v>19</v>
@@ -8431,7 +8509,7 @@
         <v>19</v>
       </c>
       <c r="G192" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H192" t="b">
         <v>0</v>
@@ -8469,7 +8547,7 @@
         <v>23</v>
       </c>
       <c r="D193" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E193" t="s">
         <v>19</v>
@@ -8516,7 +8594,7 @@
         <v>23</v>
       </c>
       <c r="D194" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="E194" t="s">
         <v>19</v>
@@ -8557,10 +8635,10 @@
         <v>7</v>
       </c>
       <c r="B196" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C196" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="D196" t="s">
         <v>18</v>
@@ -8599,7 +8677,7 @@
         <v>21</v>
       </c>
       <c r="P196" t="s">
-        <v>56</v>
+        <v>180</v>
       </c>
     </row>
     <row r="197" spans="1:16">
@@ -8613,7 +8691,7 @@
         <v>23</v>
       </c>
       <c r="D197" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="E197">
         <v>0</v>
@@ -8622,7 +8700,7 @@
         <v>19</v>
       </c>
       <c r="G197" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="H197" t="b">
         <v>0</v>
@@ -8660,7 +8738,7 @@
         <v>23</v>
       </c>
       <c r="D198" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E198" t="s">
         <v>19</v>
@@ -8669,7 +8747,7 @@
         <v>19</v>
       </c>
       <c r="G198" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H198" t="b">
         <v>0</v>
@@ -8707,7 +8785,7 @@
         <v>23</v>
       </c>
       <c r="D199" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E199" t="s">
         <v>19</v>
@@ -8754,7 +8832,7 @@
         <v>23</v>
       </c>
       <c r="D200" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E200" t="s">
         <v>19</v>
@@ -8801,7 +8879,7 @@
         <v>23</v>
       </c>
       <c r="D201" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="E201" t="s">
         <v>19</v>
@@ -8848,7 +8926,7 @@
         <v>23</v>
       </c>
       <c r="D202" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="E202" t="s">
         <v>19</v>
@@ -8895,7 +8973,7 @@
         <v>23</v>
       </c>
       <c r="D203" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="E203" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Moved SSType from Jade to Torrey
</commit_message>
<xml_diff>
--- a/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
+++ b/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
@@ -559,7 +559,7 @@
     <t>product_assigned</t>
   </si>
   <si>
-    <t>Store Reward</t>
+    <t>StoreReward</t>
   </si>
   <si>
     <t>Rewards available to loyalty customers based on which specific store points are redeemed at.</t>
@@ -7278,7 +7278,7 @@
         <v>1</v>
       </c>
       <c r="B160" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="C160" t="s">
         <v>165</v>

</xml_diff>

<commit_message>
Employee ID on order was missing in Data Dict
</commit_message>
<xml_diff>
--- a/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
+++ b/TechspireSite/TechspireSite/GeneratedFiles/DataDict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="196">
   <si>
     <t>Load Order</t>
   </si>
@@ -583,13 +583,10 @@
     <t>reward_assigned</t>
   </si>
   <si>
-    <t>OrderReward</t>
+    <t>CustomerReward</t>
   </si>
   <si>
     <t>Rewards available to a SINGLE loyalty customer to be redeemed, based on the amount of points they have accumulated to date. Available rewards that they (a single loyalty customer) has earned, based on their personal points. A points bank.</t>
-  </si>
-  <si>
-    <t>date_applied</t>
   </si>
   <si>
     <t>PointLog</t>
@@ -652,8 +649,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P209" totalsRowShown="0">
-  <autoFilter ref="A1:P209"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P208" totalsRowShown="0">
+  <autoFilter ref="A1:P208"/>
   <tableColumns count="16">
     <tableColumn id="1" name="Load Order"/>
     <tableColumn id="2" name="Owner"/>
@@ -961,7 +958,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P207"/>
+  <dimension ref="A1:P206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6148,101 +6145,101 @@
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:16">
-      <c r="A132">
-        <v>1</v>
-      </c>
-      <c r="B132" t="s">
+    <row r="131" spans="1:16">
+      <c r="A131" t="s">
+        <v>24</v>
+      </c>
+      <c r="B131" t="s">
+        <v>24</v>
+      </c>
+      <c r="C131" t="s">
+        <v>24</v>
+      </c>
+      <c r="D131" t="s">
+        <v>111</v>
+      </c>
+      <c r="E131" t="s">
+        <v>19</v>
+      </c>
+      <c r="F131" t="s">
+        <v>19</v>
+      </c>
+      <c r="G131" t="s">
+        <v>20</v>
+      </c>
+      <c r="H131" t="b">
+        <v>0</v>
+      </c>
+      <c r="I131" t="b">
+        <v>1</v>
+      </c>
+      <c r="J131" t="b">
+        <v>1</v>
+      </c>
+      <c r="K131" t="b">
+        <v>0</v>
+      </c>
+      <c r="L131" t="b">
+        <v>0</v>
+      </c>
+      <c r="M131" t="b">
+        <v>0</v>
+      </c>
+      <c r="N131" t="s">
+        <v>19</v>
+      </c>
+      <c r="P131" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16">
+      <c r="A133">
+        <v>1</v>
+      </c>
+      <c r="B133" t="s">
         <v>42</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C133" t="s">
         <v>140</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D133" t="s">
         <v>18</v>
       </c>
-      <c r="E132" t="s">
-        <v>19</v>
-      </c>
-      <c r="F132" t="s">
-        <v>19</v>
-      </c>
-      <c r="G132" t="s">
+      <c r="E133" t="s">
+        <v>19</v>
+      </c>
+      <c r="F133" t="s">
+        <v>19</v>
+      </c>
+      <c r="G133" t="s">
         <v>20</v>
       </c>
-      <c r="H132" t="b">
-        <v>1</v>
-      </c>
-      <c r="I132" t="b">
-        <v>0</v>
-      </c>
-      <c r="J132" t="b">
-        <v>1</v>
-      </c>
-      <c r="K132" t="b">
-        <v>0</v>
-      </c>
-      <c r="L132" t="b">
-        <v>0</v>
-      </c>
-      <c r="M132" t="b">
-        <v>0</v>
-      </c>
-      <c r="N132" t="s">
+      <c r="H133" t="b">
+        <v>1</v>
+      </c>
+      <c r="I133" t="b">
+        <v>0</v>
+      </c>
+      <c r="J133" t="b">
+        <v>1</v>
+      </c>
+      <c r="K133" t="b">
+        <v>0</v>
+      </c>
+      <c r="L133" t="b">
+        <v>0</v>
+      </c>
+      <c r="M133" t="b">
+        <v>0</v>
+      </c>
+      <c r="N133" t="s">
         <v>21</v>
       </c>
-      <c r="O132" t="s">
+      <c r="O133" t="s">
         <v>22</v>
       </c>
-      <c r="P132" t="s">
+      <c r="P133" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="133" spans="1:16">
-      <c r="A133" t="s">
-        <v>24</v>
-      </c>
-      <c r="B133" t="s">
-        <v>24</v>
-      </c>
-      <c r="C133" t="s">
-        <v>24</v>
-      </c>
-      <c r="D133" t="s">
-        <v>142</v>
-      </c>
-      <c r="E133" t="s">
-        <v>19</v>
-      </c>
-      <c r="F133">
-        <v>40</v>
-      </c>
-      <c r="G133" t="s">
-        <v>26</v>
-      </c>
-      <c r="H133" t="b">
-        <v>0</v>
-      </c>
-      <c r="I133" t="b">
-        <v>0</v>
-      </c>
-      <c r="J133" t="b">
-        <v>1</v>
-      </c>
-      <c r="K133" t="b">
-        <v>0</v>
-      </c>
-      <c r="L133" t="b">
-        <v>0</v>
-      </c>
-      <c r="M133" t="b">
-        <v>0</v>
-      </c>
-      <c r="N133" t="s">
-        <v>19</v>
-      </c>
-      <c r="P133" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="134" spans="1:16">
@@ -6256,13 +6253,13 @@
         <v>24</v>
       </c>
       <c r="D134" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E134" t="s">
         <v>19</v>
       </c>
       <c r="F134">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="G134" t="s">
         <v>26</v>
@@ -6274,10 +6271,10 @@
         <v>0</v>
       </c>
       <c r="J134" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K134" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L134" t="b">
         <v>0</v>
@@ -6292,101 +6289,101 @@
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
-      <c r="A136">
+    <row r="135" spans="1:16">
+      <c r="A135" t="s">
+        <v>24</v>
+      </c>
+      <c r="B135" t="s">
+        <v>24</v>
+      </c>
+      <c r="C135" t="s">
+        <v>24</v>
+      </c>
+      <c r="D135" t="s">
+        <v>143</v>
+      </c>
+      <c r="E135" t="s">
+        <v>19</v>
+      </c>
+      <c r="F135">
+        <v>200</v>
+      </c>
+      <c r="G135" t="s">
+        <v>26</v>
+      </c>
+      <c r="H135" t="b">
+        <v>0</v>
+      </c>
+      <c r="I135" t="b">
+        <v>0</v>
+      </c>
+      <c r="J135" t="b">
+        <v>0</v>
+      </c>
+      <c r="K135" t="b">
+        <v>1</v>
+      </c>
+      <c r="L135" t="b">
+        <v>0</v>
+      </c>
+      <c r="M135" t="b">
+        <v>0</v>
+      </c>
+      <c r="N135" t="s">
+        <v>19</v>
+      </c>
+      <c r="P135" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16">
+      <c r="A137">
         <v>2</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>42</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C137" t="s">
         <v>144</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D137" t="s">
         <v>18</v>
       </c>
-      <c r="E136" t="s">
-        <v>19</v>
-      </c>
-      <c r="F136" t="s">
-        <v>19</v>
-      </c>
-      <c r="G136" t="s">
+      <c r="E137" t="s">
+        <v>19</v>
+      </c>
+      <c r="F137" t="s">
+        <v>19</v>
+      </c>
+      <c r="G137" t="s">
         <v>20</v>
       </c>
-      <c r="H136" t="b">
-        <v>1</v>
-      </c>
-      <c r="I136" t="b">
-        <v>0</v>
-      </c>
-      <c r="J136" t="b">
-        <v>1</v>
-      </c>
-      <c r="K136" t="b">
-        <v>0</v>
-      </c>
-      <c r="L136" t="b">
-        <v>0</v>
-      </c>
-      <c r="M136" t="b">
-        <v>0</v>
-      </c>
-      <c r="N136" t="s">
+      <c r="H137" t="b">
+        <v>1</v>
+      </c>
+      <c r="I137" t="b">
+        <v>0</v>
+      </c>
+      <c r="J137" t="b">
+        <v>1</v>
+      </c>
+      <c r="K137" t="b">
+        <v>0</v>
+      </c>
+      <c r="L137" t="b">
+        <v>0</v>
+      </c>
+      <c r="M137" t="b">
+        <v>0</v>
+      </c>
+      <c r="N137" t="s">
         <v>21</v>
       </c>
-      <c r="O136" t="s">
+      <c r="O137" t="s">
         <v>22</v>
       </c>
-      <c r="P136" t="s">
+      <c r="P137" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="137" spans="1:16">
-      <c r="A137" t="s">
-        <v>24</v>
-      </c>
-      <c r="B137" t="s">
-        <v>24</v>
-      </c>
-      <c r="C137" t="s">
-        <v>24</v>
-      </c>
-      <c r="D137" t="s">
-        <v>146</v>
-      </c>
-      <c r="E137" t="s">
-        <v>19</v>
-      </c>
-      <c r="F137">
-        <v>80</v>
-      </c>
-      <c r="G137" t="s">
-        <v>26</v>
-      </c>
-      <c r="H137" t="b">
-        <v>0</v>
-      </c>
-      <c r="I137" t="b">
-        <v>0</v>
-      </c>
-      <c r="J137" t="b">
-        <v>1</v>
-      </c>
-      <c r="K137" t="b">
-        <v>0</v>
-      </c>
-      <c r="L137" t="b">
-        <v>0</v>
-      </c>
-      <c r="M137" t="b">
-        <v>0</v>
-      </c>
-      <c r="N137" t="s">
-        <v>19</v>
-      </c>
-      <c r="P137" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="138" spans="1:16">
@@ -6400,13 +6397,13 @@
         <v>24</v>
       </c>
       <c r="D138" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E138" t="s">
         <v>19</v>
       </c>
       <c r="F138">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G138" t="s">
         <v>26</v>
@@ -6418,10 +6415,10 @@
         <v>0</v>
       </c>
       <c r="J138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L138" t="b">
         <v>0</v>
@@ -6447,16 +6444,16 @@
         <v>24</v>
       </c>
       <c r="D139" t="s">
-        <v>148</v>
-      </c>
-      <c r="E139">
-        <v>0</v>
+        <v>147</v>
+      </c>
+      <c r="E139" t="s">
+        <v>19</v>
       </c>
       <c r="F139">
-        <v>19</v>
+        <v>200</v>
       </c>
       <c r="G139" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
       <c r="H139" t="b">
         <v>0</v>
@@ -6465,10 +6462,10 @@
         <v>0</v>
       </c>
       <c r="J139" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L139" t="b">
         <v>0</v>
@@ -6477,7 +6474,7 @@
         <v>0</v>
       </c>
       <c r="N139" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="P139" t="s">
         <v>24</v>
@@ -6494,22 +6491,22 @@
         <v>24</v>
       </c>
       <c r="D140" t="s">
-        <v>149</v>
-      </c>
-      <c r="E140" t="s">
-        <v>19</v>
-      </c>
-      <c r="F140" t="s">
+        <v>148</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
         <v>19</v>
       </c>
       <c r="G140" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="H140" t="b">
         <v>0</v>
       </c>
       <c r="I140" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J140" t="b">
         <v>1</v>
@@ -6524,7 +6521,7 @@
         <v>0</v>
       </c>
       <c r="N140" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="P140" t="s">
         <v>24</v>
@@ -6541,7 +6538,7 @@
         <v>24</v>
       </c>
       <c r="D141" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E141" t="s">
         <v>19</v>
@@ -6588,7 +6585,7 @@
         <v>24</v>
       </c>
       <c r="D142" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E142" t="s">
         <v>19</v>
@@ -6606,16 +6603,16 @@
         <v>1</v>
       </c>
       <c r="J142" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K142" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L142" t="b">
         <v>0</v>
       </c>
       <c r="M142" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N142" t="s">
         <v>19</v>
@@ -6624,71 +6621,68 @@
         <v>24</v>
       </c>
     </row>
-    <row r="144" spans="1:16">
-      <c r="A144">
+    <row r="143" spans="1:16">
+      <c r="A143" t="s">
+        <v>24</v>
+      </c>
+      <c r="B143" t="s">
+        <v>24</v>
+      </c>
+      <c r="C143" t="s">
+        <v>24</v>
+      </c>
+      <c r="D143" t="s">
+        <v>151</v>
+      </c>
+      <c r="E143" t="s">
+        <v>19</v>
+      </c>
+      <c r="F143" t="s">
+        <v>19</v>
+      </c>
+      <c r="G143" t="s">
+        <v>20</v>
+      </c>
+      <c r="H143" t="b">
+        <v>0</v>
+      </c>
+      <c r="I143" t="b">
+        <v>1</v>
+      </c>
+      <c r="J143" t="b">
+        <v>0</v>
+      </c>
+      <c r="K143" t="b">
+        <v>1</v>
+      </c>
+      <c r="L143" t="b">
+        <v>0</v>
+      </c>
+      <c r="M143" t="b">
+        <v>1</v>
+      </c>
+      <c r="N143" t="s">
+        <v>19</v>
+      </c>
+      <c r="P143" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16">
+      <c r="A145">
         <v>7</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>99</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C145" t="s">
         <v>152</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D145" t="s">
         <v>18</v>
       </c>
-      <c r="E144" t="s">
-        <v>19</v>
-      </c>
-      <c r="F144" t="s">
-        <v>19</v>
-      </c>
-      <c r="G144" t="s">
-        <v>20</v>
-      </c>
-      <c r="H144" t="b">
-        <v>1</v>
-      </c>
-      <c r="I144" t="b">
-        <v>0</v>
-      </c>
-      <c r="J144" t="b">
-        <v>1</v>
-      </c>
-      <c r="K144" t="b">
-        <v>0</v>
-      </c>
-      <c r="L144" t="b">
-        <v>0</v>
-      </c>
-      <c r="M144" t="b">
-        <v>0</v>
-      </c>
-      <c r="N144" t="s">
-        <v>21</v>
-      </c>
-      <c r="O144" t="s">
-        <v>22</v>
-      </c>
-      <c r="P144" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="145" spans="1:16">
-      <c r="A145" t="s">
-        <v>24</v>
-      </c>
-      <c r="B145" t="s">
-        <v>24</v>
-      </c>
-      <c r="C145" t="s">
-        <v>24</v>
-      </c>
-      <c r="D145" t="s">
-        <v>154</v>
-      </c>
-      <c r="E145">
-        <v>0</v>
+      <c r="E145" t="s">
+        <v>19</v>
       </c>
       <c r="F145" t="s">
         <v>19</v>
@@ -6697,7 +6691,7 @@
         <v>20</v>
       </c>
       <c r="H145" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I145" t="b">
         <v>0</v>
@@ -6715,10 +6709,13 @@
         <v>0</v>
       </c>
       <c r="N145" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="O145" t="s">
+        <v>22</v>
       </c>
       <c r="P145" t="s">
-        <v>24</v>
+        <v>153</v>
       </c>
     </row>
     <row r="146" spans="1:16">
@@ -6732,16 +6729,16 @@
         <v>24</v>
       </c>
       <c r="D146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E146">
         <v>0</v>
       </c>
-      <c r="F146">
+      <c r="F146" t="s">
         <v>19</v>
       </c>
       <c r="G146" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="H146" t="b">
         <v>0</v>
@@ -6762,7 +6759,7 @@
         <v>0</v>
       </c>
       <c r="N146" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="P146" t="s">
         <v>24</v>
@@ -6779,7 +6776,7 @@
         <v>24</v>
       </c>
       <c r="D147" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E147">
         <v>0</v>
@@ -6826,22 +6823,22 @@
         <v>24</v>
       </c>
       <c r="D148" t="s">
-        <v>157</v>
-      </c>
-      <c r="E148" t="s">
-        <v>19</v>
-      </c>
-      <c r="F148" t="s">
+        <v>156</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
         <v>19</v>
       </c>
       <c r="G148" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="H148" t="b">
         <v>0</v>
       </c>
       <c r="I148" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J148" t="b">
         <v>1</v>
@@ -6856,7 +6853,7 @@
         <v>0</v>
       </c>
       <c r="N148" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="P148" t="s">
         <v>24</v>
@@ -6873,7 +6870,7 @@
         <v>24</v>
       </c>
       <c r="D149" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E149" t="s">
         <v>19</v>
@@ -6909,101 +6906,101 @@
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="1:16">
-      <c r="A151">
+    <row r="150" spans="1:16">
+      <c r="A150" t="s">
+        <v>24</v>
+      </c>
+      <c r="B150" t="s">
+        <v>24</v>
+      </c>
+      <c r="C150" t="s">
+        <v>24</v>
+      </c>
+      <c r="D150" t="s">
+        <v>158</v>
+      </c>
+      <c r="E150" t="s">
+        <v>19</v>
+      </c>
+      <c r="F150" t="s">
+        <v>19</v>
+      </c>
+      <c r="G150" t="s">
+        <v>20</v>
+      </c>
+      <c r="H150" t="b">
+        <v>0</v>
+      </c>
+      <c r="I150" t="b">
+        <v>1</v>
+      </c>
+      <c r="J150" t="b">
+        <v>1</v>
+      </c>
+      <c r="K150" t="b">
+        <v>0</v>
+      </c>
+      <c r="L150" t="b">
+        <v>0</v>
+      </c>
+      <c r="M150" t="b">
+        <v>0</v>
+      </c>
+      <c r="N150" t="s">
+        <v>19</v>
+      </c>
+      <c r="P150" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16">
+      <c r="A152">
         <v>3</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B152" t="s">
         <v>39</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C152" t="s">
         <v>159</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D152" t="s">
         <v>18</v>
       </c>
-      <c r="E151" t="s">
-        <v>19</v>
-      </c>
-      <c r="F151" t="s">
-        <v>19</v>
-      </c>
-      <c r="G151" t="s">
+      <c r="E152" t="s">
+        <v>19</v>
+      </c>
+      <c r="F152" t="s">
+        <v>19</v>
+      </c>
+      <c r="G152" t="s">
         <v>20</v>
       </c>
-      <c r="H151" t="b">
-        <v>1</v>
-      </c>
-      <c r="I151" t="b">
-        <v>0</v>
-      </c>
-      <c r="J151" t="b">
-        <v>1</v>
-      </c>
-      <c r="K151" t="b">
-        <v>0</v>
-      </c>
-      <c r="L151" t="b">
-        <v>0</v>
-      </c>
-      <c r="M151" t="b">
-        <v>0</v>
-      </c>
-      <c r="N151" t="s">
+      <c r="H152" t="b">
+        <v>1</v>
+      </c>
+      <c r="I152" t="b">
+        <v>0</v>
+      </c>
+      <c r="J152" t="b">
+        <v>1</v>
+      </c>
+      <c r="K152" t="b">
+        <v>0</v>
+      </c>
+      <c r="L152" t="b">
+        <v>0</v>
+      </c>
+      <c r="M152" t="b">
+        <v>0</v>
+      </c>
+      <c r="N152" t="s">
         <v>21</v>
       </c>
-      <c r="O151" t="s">
+      <c r="O152" t="s">
         <v>22</v>
       </c>
-      <c r="P151" t="s">
+      <c r="P152" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="152" spans="1:16">
-      <c r="A152" t="s">
-        <v>24</v>
-      </c>
-      <c r="B152" t="s">
-        <v>24</v>
-      </c>
-      <c r="C152" t="s">
-        <v>24</v>
-      </c>
-      <c r="D152" t="s">
-        <v>161</v>
-      </c>
-      <c r="E152" t="s">
-        <v>19</v>
-      </c>
-      <c r="F152">
-        <v>80</v>
-      </c>
-      <c r="G152" t="s">
-        <v>26</v>
-      </c>
-      <c r="H152" t="b">
-        <v>0</v>
-      </c>
-      <c r="I152" t="b">
-        <v>0</v>
-      </c>
-      <c r="J152" t="b">
-        <v>1</v>
-      </c>
-      <c r="K152" t="b">
-        <v>0</v>
-      </c>
-      <c r="L152" t="b">
-        <v>0</v>
-      </c>
-      <c r="M152" t="b">
-        <v>0</v>
-      </c>
-      <c r="N152" t="s">
-        <v>19</v>
-      </c>
-      <c r="P152" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="153" spans="1:16">
@@ -7017,13 +7014,13 @@
         <v>24</v>
       </c>
       <c r="D153" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E153" t="s">
         <v>19</v>
       </c>
       <c r="F153">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="G153" t="s">
         <v>26</v>
@@ -7035,10 +7032,10 @@
         <v>0</v>
       </c>
       <c r="J153" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K153" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L153" t="b">
         <v>0</v>
@@ -7064,28 +7061,28 @@
         <v>24</v>
       </c>
       <c r="D154" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E154" t="s">
         <v>19</v>
       </c>
-      <c r="F154" t="s">
-        <v>19</v>
+      <c r="F154">
+        <v>200</v>
       </c>
       <c r="G154" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H154" t="b">
         <v>0</v>
       </c>
       <c r="I154" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J154" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K154" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L154" t="b">
         <v>0</v>
@@ -7111,10 +7108,10 @@
         <v>24</v>
       </c>
       <c r="D155" t="s">
-        <v>164</v>
-      </c>
-      <c r="E155">
-        <v>0</v>
+        <v>163</v>
+      </c>
+      <c r="E155" t="s">
+        <v>19</v>
       </c>
       <c r="F155" t="s">
         <v>19</v>
@@ -7126,7 +7123,7 @@
         <v>0</v>
       </c>
       <c r="I155" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J155" t="b">
         <v>1</v>
@@ -7158,7 +7155,7 @@
         <v>24</v>
       </c>
       <c r="D156" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E156">
         <v>0</v>
@@ -7176,10 +7173,10 @@
         <v>0</v>
       </c>
       <c r="J156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K156" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L156" t="b">
         <v>0</v>
@@ -7205,16 +7202,16 @@
         <v>24</v>
       </c>
       <c r="D157" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="E157">
         <v>0</v>
       </c>
-      <c r="F157">
+      <c r="F157" t="s">
         <v>19</v>
       </c>
       <c r="G157" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="H157" t="b">
         <v>0</v>
@@ -7223,10 +7220,10 @@
         <v>0</v>
       </c>
       <c r="J157" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K157" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L157" t="b">
         <v>0</v>
@@ -7235,7 +7232,7 @@
         <v>0</v>
       </c>
       <c r="N157" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="P157" t="s">
         <v>24</v>
@@ -7252,37 +7249,37 @@
         <v>24</v>
       </c>
       <c r="D158" t="s">
-        <v>166</v>
-      </c>
-      <c r="E158" t="s">
-        <v>19</v>
-      </c>
-      <c r="F158" t="s">
+        <v>138</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
         <v>19</v>
       </c>
       <c r="G158" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="H158" t="b">
         <v>0</v>
       </c>
       <c r="I158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J158" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L158" t="b">
         <v>0</v>
       </c>
       <c r="M158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N158" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="P158" t="s">
         <v>24</v>
@@ -7299,7 +7296,7 @@
         <v>24</v>
       </c>
       <c r="D159" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="E159" t="s">
         <v>19</v>
@@ -7346,7 +7343,7 @@
         <v>24</v>
       </c>
       <c r="D160" t="s">
-        <v>167</v>
+        <v>104</v>
       </c>
       <c r="E160" t="s">
         <v>19</v>
@@ -7355,25 +7352,25 @@
         <v>19</v>
       </c>
       <c r="G160" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="H160" t="b">
         <v>0</v>
       </c>
       <c r="I160" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J160" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K160" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L160" t="b">
         <v>0</v>
       </c>
       <c r="M160" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N160" t="s">
         <v>19</v>
@@ -7393,7 +7390,7 @@
         <v>24</v>
       </c>
       <c r="D161" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E161" t="s">
         <v>19</v>
@@ -7411,10 +7408,10 @@
         <v>0</v>
       </c>
       <c r="J161" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K161" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L161" t="b">
         <v>0</v>
@@ -7429,101 +7426,101 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:16">
-      <c r="A163">
-        <v>1</v>
-      </c>
-      <c r="B163" t="s">
+    <row r="162" spans="1:16">
+      <c r="A162" t="s">
+        <v>24</v>
+      </c>
+      <c r="B162" t="s">
+        <v>24</v>
+      </c>
+      <c r="C162" t="s">
+        <v>24</v>
+      </c>
+      <c r="D162" t="s">
+        <v>168</v>
+      </c>
+      <c r="E162" t="s">
+        <v>19</v>
+      </c>
+      <c r="F162" t="s">
+        <v>19</v>
+      </c>
+      <c r="G162" t="s">
+        <v>91</v>
+      </c>
+      <c r="H162" t="b">
+        <v>0</v>
+      </c>
+      <c r="I162" t="b">
+        <v>0</v>
+      </c>
+      <c r="J162" t="b">
+        <v>0</v>
+      </c>
+      <c r="K162" t="b">
+        <v>1</v>
+      </c>
+      <c r="L162" t="b">
+        <v>0</v>
+      </c>
+      <c r="M162" t="b">
+        <v>0</v>
+      </c>
+      <c r="N162" t="s">
+        <v>19</v>
+      </c>
+      <c r="P162" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16">
+      <c r="A164">
+        <v>1</v>
+      </c>
+      <c r="B164" t="s">
         <v>130</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C164" t="s">
         <v>169</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D164" t="s">
         <v>18</v>
       </c>
-      <c r="E163" t="s">
-        <v>19</v>
-      </c>
-      <c r="F163" t="s">
-        <v>19</v>
-      </c>
-      <c r="G163" t="s">
+      <c r="E164" t="s">
+        <v>19</v>
+      </c>
+      <c r="F164" t="s">
+        <v>19</v>
+      </c>
+      <c r="G164" t="s">
         <v>20</v>
       </c>
-      <c r="H163" t="b">
-        <v>1</v>
-      </c>
-      <c r="I163" t="b">
-        <v>0</v>
-      </c>
-      <c r="J163" t="b">
-        <v>1</v>
-      </c>
-      <c r="K163" t="b">
-        <v>0</v>
-      </c>
-      <c r="L163" t="b">
-        <v>0</v>
-      </c>
-      <c r="M163" t="b">
-        <v>0</v>
-      </c>
-      <c r="N163" t="s">
+      <c r="H164" t="b">
+        <v>1</v>
+      </c>
+      <c r="I164" t="b">
+        <v>0</v>
+      </c>
+      <c r="J164" t="b">
+        <v>1</v>
+      </c>
+      <c r="K164" t="b">
+        <v>0</v>
+      </c>
+      <c r="L164" t="b">
+        <v>0</v>
+      </c>
+      <c r="M164" t="b">
+        <v>0</v>
+      </c>
+      <c r="N164" t="s">
         <v>21</v>
       </c>
-      <c r="O163" t="s">
+      <c r="O164" t="s">
         <v>22</v>
       </c>
-      <c r="P163" t="s">
+      <c r="P164" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="164" spans="1:16">
-      <c r="A164" t="s">
-        <v>24</v>
-      </c>
-      <c r="B164" t="s">
-        <v>24</v>
-      </c>
-      <c r="C164" t="s">
-        <v>24</v>
-      </c>
-      <c r="D164" t="s">
-        <v>171</v>
-      </c>
-      <c r="E164" t="s">
-        <v>19</v>
-      </c>
-      <c r="F164">
-        <v>40</v>
-      </c>
-      <c r="G164" t="s">
-        <v>26</v>
-      </c>
-      <c r="H164" t="b">
-        <v>0</v>
-      </c>
-      <c r="I164" t="b">
-        <v>0</v>
-      </c>
-      <c r="J164" t="b">
-        <v>1</v>
-      </c>
-      <c r="K164" t="b">
-        <v>0</v>
-      </c>
-      <c r="L164" t="b">
-        <v>0</v>
-      </c>
-      <c r="M164" t="b">
-        <v>0</v>
-      </c>
-      <c r="N164" t="s">
-        <v>19</v>
-      </c>
-      <c r="P164" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="165" spans="1:16">
@@ -7537,13 +7534,13 @@
         <v>24</v>
       </c>
       <c r="D165" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E165" t="s">
         <v>19</v>
       </c>
       <c r="F165">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="G165" t="s">
         <v>26</v>
@@ -7555,10 +7552,10 @@
         <v>0</v>
       </c>
       <c r="J165" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K165" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L165" t="b">
         <v>0</v>
@@ -7573,101 +7570,101 @@
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:16">
-      <c r="A167">
+    <row r="166" spans="1:16">
+      <c r="A166" t="s">
+        <v>24</v>
+      </c>
+      <c r="B166" t="s">
+        <v>24</v>
+      </c>
+      <c r="C166" t="s">
+        <v>24</v>
+      </c>
+      <c r="D166" t="s">
+        <v>172</v>
+      </c>
+      <c r="E166" t="s">
+        <v>19</v>
+      </c>
+      <c r="F166">
+        <v>200</v>
+      </c>
+      <c r="G166" t="s">
+        <v>26</v>
+      </c>
+      <c r="H166" t="b">
+        <v>0</v>
+      </c>
+      <c r="I166" t="b">
+        <v>0</v>
+      </c>
+      <c r="J166" t="b">
+        <v>0</v>
+      </c>
+      <c r="K166" t="b">
+        <v>1</v>
+      </c>
+      <c r="L166" t="b">
+        <v>0</v>
+      </c>
+      <c r="M166" t="b">
+        <v>0</v>
+      </c>
+      <c r="N166" t="s">
+        <v>19</v>
+      </c>
+      <c r="P166" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16">
+      <c r="A168">
         <v>5</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B168" t="s">
         <v>173</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C168" t="s">
         <v>174</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D168" t="s">
         <v>18</v>
       </c>
-      <c r="E167" t="s">
-        <v>19</v>
-      </c>
-      <c r="F167" t="s">
-        <v>19</v>
-      </c>
-      <c r="G167" t="s">
+      <c r="E168" t="s">
+        <v>19</v>
+      </c>
+      <c r="F168" t="s">
+        <v>19</v>
+      </c>
+      <c r="G168" t="s">
         <v>20</v>
       </c>
-      <c r="H167" t="b">
-        <v>1</v>
-      </c>
-      <c r="I167" t="b">
-        <v>0</v>
-      </c>
-      <c r="J167" t="b">
-        <v>1</v>
-      </c>
-      <c r="K167" t="b">
-        <v>0</v>
-      </c>
-      <c r="L167" t="b">
-        <v>0</v>
-      </c>
-      <c r="M167" t="b">
-        <v>0</v>
-      </c>
-      <c r="N167" t="s">
+      <c r="H168" t="b">
+        <v>1</v>
+      </c>
+      <c r="I168" t="b">
+        <v>0</v>
+      </c>
+      <c r="J168" t="b">
+        <v>1</v>
+      </c>
+      <c r="K168" t="b">
+        <v>0</v>
+      </c>
+      <c r="L168" t="b">
+        <v>0</v>
+      </c>
+      <c r="M168" t="b">
+        <v>0</v>
+      </c>
+      <c r="N168" t="s">
         <v>21</v>
       </c>
-      <c r="O167" t="s">
+      <c r="O168" t="s">
         <v>22</v>
       </c>
-      <c r="P167" t="s">
+      <c r="P168" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="168" spans="1:16">
-      <c r="A168" t="s">
-        <v>24</v>
-      </c>
-      <c r="B168" t="s">
-        <v>24</v>
-      </c>
-      <c r="C168" t="s">
-        <v>24</v>
-      </c>
-      <c r="D168" t="s">
-        <v>176</v>
-      </c>
-      <c r="E168" t="s">
-        <v>19</v>
-      </c>
-      <c r="F168">
-        <v>60</v>
-      </c>
-      <c r="G168" t="s">
-        <v>26</v>
-      </c>
-      <c r="H168" t="b">
-        <v>0</v>
-      </c>
-      <c r="I168" t="b">
-        <v>0</v>
-      </c>
-      <c r="J168" t="b">
-        <v>1</v>
-      </c>
-      <c r="K168" t="b">
-        <v>0</v>
-      </c>
-      <c r="L168" t="b">
-        <v>0</v>
-      </c>
-      <c r="M168" t="b">
-        <v>0</v>
-      </c>
-      <c r="N168" t="s">
-        <v>19</v>
-      </c>
-      <c r="P168" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="169" spans="1:16">
@@ -7681,22 +7678,22 @@
         <v>24</v>
       </c>
       <c r="D169" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="E169" t="s">
         <v>19</v>
       </c>
-      <c r="F169" t="s">
-        <v>19</v>
+      <c r="F169">
+        <v>60</v>
       </c>
       <c r="G169" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H169" t="b">
         <v>0</v>
       </c>
       <c r="I169" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J169" t="b">
         <v>1</v>
@@ -7728,7 +7725,7 @@
         <v>24</v>
       </c>
       <c r="D170" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="E170" t="s">
         <v>19</v>
@@ -7775,137 +7772,137 @@
         <v>24</v>
       </c>
       <c r="D171" t="s">
+        <v>177</v>
+      </c>
+      <c r="E171" t="s">
+        <v>19</v>
+      </c>
+      <c r="F171" t="s">
+        <v>19</v>
+      </c>
+      <c r="G171" t="s">
+        <v>20</v>
+      </c>
+      <c r="H171" t="b">
+        <v>0</v>
+      </c>
+      <c r="I171" t="b">
+        <v>1</v>
+      </c>
+      <c r="J171" t="b">
+        <v>1</v>
+      </c>
+      <c r="K171" t="b">
+        <v>0</v>
+      </c>
+      <c r="L171" t="b">
+        <v>0</v>
+      </c>
+      <c r="M171" t="b">
+        <v>0</v>
+      </c>
+      <c r="N171" t="s">
+        <v>19</v>
+      </c>
+      <c r="P171" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16">
+      <c r="A172" t="s">
+        <v>24</v>
+      </c>
+      <c r="B172" t="s">
+        <v>24</v>
+      </c>
+      <c r="C172" t="s">
+        <v>24</v>
+      </c>
+      <c r="D172" t="s">
         <v>167</v>
       </c>
-      <c r="E171" t="s">
-        <v>19</v>
-      </c>
-      <c r="F171" t="s">
-        <v>19</v>
-      </c>
-      <c r="G171" t="s">
+      <c r="E172" t="s">
+        <v>19</v>
+      </c>
+      <c r="F172" t="s">
+        <v>19</v>
+      </c>
+      <c r="G172" t="s">
         <v>91</v>
       </c>
-      <c r="H171" t="b">
-        <v>0</v>
-      </c>
-      <c r="I171" t="b">
-        <v>0</v>
-      </c>
-      <c r="J171" t="b">
-        <v>1</v>
-      </c>
-      <c r="K171" t="b">
-        <v>0</v>
-      </c>
-      <c r="L171" t="b">
-        <v>0</v>
-      </c>
-      <c r="M171" t="b">
-        <v>0</v>
-      </c>
-      <c r="N171" t="s">
-        <v>19</v>
-      </c>
-      <c r="P171" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="173" spans="1:16">
-      <c r="A173">
+      <c r="H172" t="b">
+        <v>0</v>
+      </c>
+      <c r="I172" t="b">
+        <v>0</v>
+      </c>
+      <c r="J172" t="b">
+        <v>1</v>
+      </c>
+      <c r="K172" t="b">
+        <v>0</v>
+      </c>
+      <c r="L172" t="b">
+        <v>0</v>
+      </c>
+      <c r="M172" t="b">
+        <v>0</v>
+      </c>
+      <c r="N172" t="s">
+        <v>19</v>
+      </c>
+      <c r="P172" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16">
+      <c r="A174">
         <v>5</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B174" t="s">
         <v>173</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C174" t="s">
         <v>178</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D174" t="s">
         <v>18</v>
       </c>
-      <c r="E173" t="s">
-        <v>19</v>
-      </c>
-      <c r="F173" t="s">
-        <v>19</v>
-      </c>
-      <c r="G173" t="s">
+      <c r="E174" t="s">
+        <v>19</v>
+      </c>
+      <c r="F174" t="s">
+        <v>19</v>
+      </c>
+      <c r="G174" t="s">
         <v>20</v>
       </c>
-      <c r="H173" t="b">
-        <v>1</v>
-      </c>
-      <c r="I173" t="b">
-        <v>0</v>
-      </c>
-      <c r="J173" t="b">
-        <v>1</v>
-      </c>
-      <c r="K173" t="b">
-        <v>0</v>
-      </c>
-      <c r="L173" t="b">
-        <v>0</v>
-      </c>
-      <c r="M173" t="b">
-        <v>0</v>
-      </c>
-      <c r="N173" t="s">
+      <c r="H174" t="b">
+        <v>1</v>
+      </c>
+      <c r="I174" t="b">
+        <v>0</v>
+      </c>
+      <c r="J174" t="b">
+        <v>1</v>
+      </c>
+      <c r="K174" t="b">
+        <v>0</v>
+      </c>
+      <c r="L174" t="b">
+        <v>0</v>
+      </c>
+      <c r="M174" t="b">
+        <v>0</v>
+      </c>
+      <c r="N174" t="s">
         <v>21</v>
       </c>
-      <c r="O173" t="s">
+      <c r="O174" t="s">
         <v>22</v>
       </c>
-      <c r="P173" t="s">
+      <c r="P174" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="174" spans="1:16">
-      <c r="A174" t="s">
-        <v>24</v>
-      </c>
-      <c r="B174" t="s">
-        <v>24</v>
-      </c>
-      <c r="C174" t="s">
-        <v>24</v>
-      </c>
-      <c r="D174" t="s">
-        <v>176</v>
-      </c>
-      <c r="E174" t="s">
-        <v>19</v>
-      </c>
-      <c r="F174">
-        <v>60</v>
-      </c>
-      <c r="G174" t="s">
-        <v>26</v>
-      </c>
-      <c r="H174" t="b">
-        <v>0</v>
-      </c>
-      <c r="I174" t="b">
-        <v>0</v>
-      </c>
-      <c r="J174" t="b">
-        <v>1</v>
-      </c>
-      <c r="K174" t="b">
-        <v>0</v>
-      </c>
-      <c r="L174" t="b">
-        <v>0</v>
-      </c>
-      <c r="M174" t="b">
-        <v>0</v>
-      </c>
-      <c r="N174" t="s">
-        <v>19</v>
-      </c>
-      <c r="P174" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="175" spans="1:16">
@@ -7919,22 +7916,22 @@
         <v>24</v>
       </c>
       <c r="D175" t="s">
-        <v>111</v>
+        <v>176</v>
       </c>
       <c r="E175" t="s">
         <v>19</v>
       </c>
-      <c r="F175" t="s">
-        <v>19</v>
+      <c r="F175">
+        <v>60</v>
       </c>
       <c r="G175" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H175" t="b">
         <v>0</v>
       </c>
       <c r="I175" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J175" t="b">
         <v>1</v>
@@ -7966,7 +7963,7 @@
         <v>24</v>
       </c>
       <c r="D176" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
       <c r="E176" t="s">
         <v>19</v>
@@ -8013,137 +8010,137 @@
         <v>24</v>
       </c>
       <c r="D177" t="s">
+        <v>177</v>
+      </c>
+      <c r="E177" t="s">
+        <v>19</v>
+      </c>
+      <c r="F177" t="s">
+        <v>19</v>
+      </c>
+      <c r="G177" t="s">
+        <v>20</v>
+      </c>
+      <c r="H177" t="b">
+        <v>0</v>
+      </c>
+      <c r="I177" t="b">
+        <v>1</v>
+      </c>
+      <c r="J177" t="b">
+        <v>1</v>
+      </c>
+      <c r="K177" t="b">
+        <v>0</v>
+      </c>
+      <c r="L177" t="b">
+        <v>0</v>
+      </c>
+      <c r="M177" t="b">
+        <v>0</v>
+      </c>
+      <c r="N177" t="s">
+        <v>19</v>
+      </c>
+      <c r="P177" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16">
+      <c r="A178" t="s">
+        <v>24</v>
+      </c>
+      <c r="B178" t="s">
+        <v>24</v>
+      </c>
+      <c r="C178" t="s">
+        <v>24</v>
+      </c>
+      <c r="D178" t="s">
         <v>167</v>
       </c>
-      <c r="E177" t="s">
-        <v>19</v>
-      </c>
-      <c r="F177" t="s">
-        <v>19</v>
-      </c>
-      <c r="G177" t="s">
+      <c r="E178" t="s">
+        <v>19</v>
+      </c>
+      <c r="F178" t="s">
+        <v>19</v>
+      </c>
+      <c r="G178" t="s">
         <v>91</v>
       </c>
-      <c r="H177" t="b">
-        <v>0</v>
-      </c>
-      <c r="I177" t="b">
-        <v>0</v>
-      </c>
-      <c r="J177" t="b">
-        <v>1</v>
-      </c>
-      <c r="K177" t="b">
-        <v>0</v>
-      </c>
-      <c r="L177" t="b">
-        <v>0</v>
-      </c>
-      <c r="M177" t="b">
-        <v>0</v>
-      </c>
-      <c r="N177" t="s">
-        <v>19</v>
-      </c>
-      <c r="P177" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="179" spans="1:16">
-      <c r="A179">
+      <c r="H178" t="b">
+        <v>0</v>
+      </c>
+      <c r="I178" t="b">
+        <v>0</v>
+      </c>
+      <c r="J178" t="b">
+        <v>1</v>
+      </c>
+      <c r="K178" t="b">
+        <v>0</v>
+      </c>
+      <c r="L178" t="b">
+        <v>0</v>
+      </c>
+      <c r="M178" t="b">
+        <v>0</v>
+      </c>
+      <c r="N178" t="s">
+        <v>19</v>
+      </c>
+      <c r="P178" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16">
+      <c r="A180">
         <v>6</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B180" t="s">
         <v>53</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C180" t="s">
         <v>180</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D180" t="s">
         <v>18</v>
       </c>
-      <c r="E179" t="s">
-        <v>19</v>
-      </c>
-      <c r="F179" t="s">
-        <v>19</v>
-      </c>
-      <c r="G179" t="s">
+      <c r="E180" t="s">
+        <v>19</v>
+      </c>
+      <c r="F180" t="s">
+        <v>19</v>
+      </c>
+      <c r="G180" t="s">
         <v>20</v>
       </c>
-      <c r="H179" t="b">
-        <v>1</v>
-      </c>
-      <c r="I179" t="b">
-        <v>0</v>
-      </c>
-      <c r="J179" t="b">
-        <v>1</v>
-      </c>
-      <c r="K179" t="b">
-        <v>0</v>
-      </c>
-      <c r="L179" t="b">
-        <v>0</v>
-      </c>
-      <c r="M179" t="b">
-        <v>0</v>
-      </c>
-      <c r="N179" t="s">
+      <c r="H180" t="b">
+        <v>1</v>
+      </c>
+      <c r="I180" t="b">
+        <v>0</v>
+      </c>
+      <c r="J180" t="b">
+        <v>1</v>
+      </c>
+      <c r="K180" t="b">
+        <v>0</v>
+      </c>
+      <c r="L180" t="b">
+        <v>0</v>
+      </c>
+      <c r="M180" t="b">
+        <v>0</v>
+      </c>
+      <c r="N180" t="s">
         <v>21</v>
       </c>
-      <c r="O179" t="s">
+      <c r="O180" t="s">
         <v>22</v>
       </c>
-      <c r="P179" t="s">
+      <c r="P180" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="180" spans="1:16">
-      <c r="A180" t="s">
-        <v>24</v>
-      </c>
-      <c r="B180" t="s">
-        <v>24</v>
-      </c>
-      <c r="C180" t="s">
-        <v>24</v>
-      </c>
-      <c r="D180" t="s">
-        <v>176</v>
-      </c>
-      <c r="E180" t="s">
-        <v>19</v>
-      </c>
-      <c r="F180">
-        <v>60</v>
-      </c>
-      <c r="G180" t="s">
-        <v>26</v>
-      </c>
-      <c r="H180" t="b">
-        <v>0</v>
-      </c>
-      <c r="I180" t="b">
-        <v>0</v>
-      </c>
-      <c r="J180" t="b">
-        <v>1</v>
-      </c>
-      <c r="K180" t="b">
-        <v>0</v>
-      </c>
-      <c r="L180" t="b">
-        <v>0</v>
-      </c>
-      <c r="M180" t="b">
-        <v>0</v>
-      </c>
-      <c r="N180" t="s">
-        <v>19</v>
-      </c>
-      <c r="P180" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="181" spans="1:16">
@@ -8157,22 +8154,22 @@
         <v>24</v>
       </c>
       <c r="D181" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E181" t="s">
         <v>19</v>
       </c>
-      <c r="F181" t="s">
-        <v>19</v>
+      <c r="F181">
+        <v>60</v>
       </c>
       <c r="G181" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H181" t="b">
         <v>0</v>
       </c>
       <c r="I181" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J181" t="b">
         <v>1</v>
@@ -8204,7 +8201,7 @@
         <v>24</v>
       </c>
       <c r="D182" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="E182" t="s">
         <v>19</v>
@@ -8251,104 +8248,101 @@
         <v>24</v>
       </c>
       <c r="D183" t="s">
+        <v>115</v>
+      </c>
+      <c r="E183" t="s">
+        <v>19</v>
+      </c>
+      <c r="F183" t="s">
+        <v>19</v>
+      </c>
+      <c r="G183" t="s">
+        <v>20</v>
+      </c>
+      <c r="H183" t="b">
+        <v>0</v>
+      </c>
+      <c r="I183" t="b">
+        <v>1</v>
+      </c>
+      <c r="J183" t="b">
+        <v>1</v>
+      </c>
+      <c r="K183" t="b">
+        <v>0</v>
+      </c>
+      <c r="L183" t="b">
+        <v>0</v>
+      </c>
+      <c r="M183" t="b">
+        <v>0</v>
+      </c>
+      <c r="N183" t="s">
+        <v>19</v>
+      </c>
+      <c r="P183" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16">
+      <c r="A184" t="s">
+        <v>24</v>
+      </c>
+      <c r="B184" t="s">
+        <v>24</v>
+      </c>
+      <c r="C184" t="s">
+        <v>24</v>
+      </c>
+      <c r="D184" t="s">
         <v>167</v>
       </c>
-      <c r="E183" t="s">
-        <v>19</v>
-      </c>
-      <c r="F183" t="s">
-        <v>19</v>
-      </c>
-      <c r="G183" t="s">
+      <c r="E184" t="s">
+        <v>19</v>
+      </c>
+      <c r="F184" t="s">
+        <v>19</v>
+      </c>
+      <c r="G184" t="s">
         <v>91</v>
       </c>
-      <c r="H183" t="b">
-        <v>0</v>
-      </c>
-      <c r="I183" t="b">
-        <v>0</v>
-      </c>
-      <c r="J183" t="b">
-        <v>1</v>
-      </c>
-      <c r="K183" t="b">
-        <v>0</v>
-      </c>
-      <c r="L183" t="b">
-        <v>0</v>
-      </c>
-      <c r="M183" t="b">
-        <v>0</v>
-      </c>
-      <c r="N183" t="s">
-        <v>19</v>
-      </c>
-      <c r="P183" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="185" spans="1:16">
-      <c r="A185">
+      <c r="H184" t="b">
+        <v>0</v>
+      </c>
+      <c r="I184" t="b">
+        <v>0</v>
+      </c>
+      <c r="J184" t="b">
+        <v>1</v>
+      </c>
+      <c r="K184" t="b">
+        <v>0</v>
+      </c>
+      <c r="L184" t="b">
+        <v>0</v>
+      </c>
+      <c r="M184" t="b">
+        <v>0</v>
+      </c>
+      <c r="N184" t="s">
+        <v>19</v>
+      </c>
+      <c r="P184" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16">
+      <c r="A186">
         <v>5</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B186" t="s">
         <v>130</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C186" t="s">
         <v>182</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D186" t="s">
         <v>18</v>
-      </c>
-      <c r="E185" t="s">
-        <v>19</v>
-      </c>
-      <c r="F185" t="s">
-        <v>19</v>
-      </c>
-      <c r="G185" t="s">
-        <v>20</v>
-      </c>
-      <c r="H185" t="b">
-        <v>1</v>
-      </c>
-      <c r="I185" t="b">
-        <v>0</v>
-      </c>
-      <c r="J185" t="b">
-        <v>1</v>
-      </c>
-      <c r="K185" t="b">
-        <v>0</v>
-      </c>
-      <c r="L185" t="b">
-        <v>0</v>
-      </c>
-      <c r="M185" t="b">
-        <v>0</v>
-      </c>
-      <c r="N185" t="s">
-        <v>21</v>
-      </c>
-      <c r="O185" t="s">
-        <v>22</v>
-      </c>
-      <c r="P185" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="186" spans="1:16">
-      <c r="A186" t="s">
-        <v>24</v>
-      </c>
-      <c r="B186" t="s">
-        <v>24</v>
-      </c>
-      <c r="C186" t="s">
-        <v>24</v>
-      </c>
-      <c r="D186" t="s">
-        <v>157</v>
       </c>
       <c r="E186" t="s">
         <v>19</v>
@@ -8360,10 +8354,10 @@
         <v>20</v>
       </c>
       <c r="H186" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I186" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J186" t="b">
         <v>1</v>
@@ -8378,10 +8372,13 @@
         <v>0</v>
       </c>
       <c r="N186" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="O186" t="s">
+        <v>22</v>
       </c>
       <c r="P186" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
     </row>
     <row r="187" spans="1:16">
@@ -8395,7 +8392,7 @@
         <v>24</v>
       </c>
       <c r="D187" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="E187" t="s">
         <v>19</v>
@@ -8442,104 +8439,101 @@
         <v>24</v>
       </c>
       <c r="D188" t="s">
+        <v>128</v>
+      </c>
+      <c r="E188" t="s">
+        <v>19</v>
+      </c>
+      <c r="F188" t="s">
+        <v>19</v>
+      </c>
+      <c r="G188" t="s">
+        <v>20</v>
+      </c>
+      <c r="H188" t="b">
+        <v>0</v>
+      </c>
+      <c r="I188" t="b">
+        <v>1</v>
+      </c>
+      <c r="J188" t="b">
+        <v>1</v>
+      </c>
+      <c r="K188" t="b">
+        <v>0</v>
+      </c>
+      <c r="L188" t="b">
+        <v>0</v>
+      </c>
+      <c r="M188" t="b">
+        <v>0</v>
+      </c>
+      <c r="N188" t="s">
+        <v>19</v>
+      </c>
+      <c r="P188" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16">
+      <c r="A189" t="s">
+        <v>24</v>
+      </c>
+      <c r="B189" t="s">
+        <v>24</v>
+      </c>
+      <c r="C189" t="s">
+        <v>24</v>
+      </c>
+      <c r="D189" t="s">
         <v>184</v>
       </c>
-      <c r="E188" t="s">
-        <v>19</v>
-      </c>
-      <c r="F188" t="s">
-        <v>19</v>
-      </c>
-      <c r="G188" t="s">
+      <c r="E189" t="s">
+        <v>19</v>
+      </c>
+      <c r="F189" t="s">
+        <v>19</v>
+      </c>
+      <c r="G189" t="s">
         <v>91</v>
       </c>
-      <c r="H188" t="b">
-        <v>0</v>
-      </c>
-      <c r="I188" t="b">
-        <v>0</v>
-      </c>
-      <c r="J188" t="b">
-        <v>1</v>
-      </c>
-      <c r="K188" t="b">
-        <v>0</v>
-      </c>
-      <c r="L188" t="b">
-        <v>0</v>
-      </c>
-      <c r="M188" t="b">
-        <v>0</v>
-      </c>
-      <c r="N188" t="s">
-        <v>19</v>
-      </c>
-      <c r="P188" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="190" spans="1:16">
-      <c r="A190">
+      <c r="H189" t="b">
+        <v>0</v>
+      </c>
+      <c r="I189" t="b">
+        <v>0</v>
+      </c>
+      <c r="J189" t="b">
+        <v>1</v>
+      </c>
+      <c r="K189" t="b">
+        <v>0</v>
+      </c>
+      <c r="L189" t="b">
+        <v>0</v>
+      </c>
+      <c r="M189" t="b">
+        <v>0</v>
+      </c>
+      <c r="N189" t="s">
+        <v>19</v>
+      </c>
+      <c r="P189" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16">
+      <c r="A191">
         <v>5</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B191" t="s">
         <v>173</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C191" t="s">
         <v>185</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D191" t="s">
         <v>18</v>
-      </c>
-      <c r="E190" t="s">
-        <v>19</v>
-      </c>
-      <c r="F190" t="s">
-        <v>19</v>
-      </c>
-      <c r="G190" t="s">
-        <v>20</v>
-      </c>
-      <c r="H190" t="b">
-        <v>1</v>
-      </c>
-      <c r="I190" t="b">
-        <v>0</v>
-      </c>
-      <c r="J190" t="b">
-        <v>1</v>
-      </c>
-      <c r="K190" t="b">
-        <v>0</v>
-      </c>
-      <c r="L190" t="b">
-        <v>0</v>
-      </c>
-      <c r="M190" t="b">
-        <v>0</v>
-      </c>
-      <c r="N190" t="s">
-        <v>21</v>
-      </c>
-      <c r="O190" t="s">
-        <v>22</v>
-      </c>
-      <c r="P190" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="191" spans="1:16">
-      <c r="A191" t="s">
-        <v>24</v>
-      </c>
-      <c r="B191" t="s">
-        <v>24</v>
-      </c>
-      <c r="C191" t="s">
-        <v>24</v>
-      </c>
-      <c r="D191" t="s">
-        <v>187</v>
       </c>
       <c r="E191" t="s">
         <v>19</v>
@@ -8551,10 +8545,10 @@
         <v>20</v>
       </c>
       <c r="H191" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I191" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J191" t="b">
         <v>1</v>
@@ -8569,10 +8563,13 @@
         <v>0</v>
       </c>
       <c r="N191" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="O191" t="s">
+        <v>22</v>
       </c>
       <c r="P191" t="s">
-        <v>24</v>
+        <v>186</v>
       </c>
     </row>
     <row r="192" spans="1:16">
@@ -8586,7 +8583,7 @@
         <v>24</v>
       </c>
       <c r="D192" t="s">
-        <v>128</v>
+        <v>187</v>
       </c>
       <c r="E192" t="s">
         <v>19</v>
@@ -8633,137 +8630,137 @@
         <v>24</v>
       </c>
       <c r="D193" t="s">
+        <v>128</v>
+      </c>
+      <c r="E193" t="s">
+        <v>19</v>
+      </c>
+      <c r="F193" t="s">
+        <v>19</v>
+      </c>
+      <c r="G193" t="s">
+        <v>20</v>
+      </c>
+      <c r="H193" t="b">
+        <v>0</v>
+      </c>
+      <c r="I193" t="b">
+        <v>1</v>
+      </c>
+      <c r="J193" t="b">
+        <v>1</v>
+      </c>
+      <c r="K193" t="b">
+        <v>0</v>
+      </c>
+      <c r="L193" t="b">
+        <v>0</v>
+      </c>
+      <c r="M193" t="b">
+        <v>0</v>
+      </c>
+      <c r="N193" t="s">
+        <v>19</v>
+      </c>
+      <c r="P193" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16">
+      <c r="A194" t="s">
+        <v>24</v>
+      </c>
+      <c r="B194" t="s">
+        <v>24</v>
+      </c>
+      <c r="C194" t="s">
+        <v>24</v>
+      </c>
+      <c r="D194" t="s">
         <v>188</v>
       </c>
-      <c r="E193" t="s">
-        <v>19</v>
-      </c>
-      <c r="F193" t="s">
-        <v>19</v>
-      </c>
-      <c r="G193" t="s">
+      <c r="E194" t="s">
+        <v>19</v>
+      </c>
+      <c r="F194" t="s">
+        <v>19</v>
+      </c>
+      <c r="G194" t="s">
         <v>91</v>
       </c>
-      <c r="H193" t="b">
-        <v>0</v>
-      </c>
-      <c r="I193" t="b">
-        <v>0</v>
-      </c>
-      <c r="J193" t="b">
-        <v>1</v>
-      </c>
-      <c r="K193" t="b">
-        <v>0</v>
-      </c>
-      <c r="L193" t="b">
-        <v>0</v>
-      </c>
-      <c r="M193" t="b">
-        <v>0</v>
-      </c>
-      <c r="N193" t="s">
-        <v>19</v>
-      </c>
-      <c r="P193" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="195" spans="1:16">
-      <c r="A195">
-        <v>6</v>
-      </c>
-      <c r="B195" t="s">
+      <c r="H194" t="b">
+        <v>0</v>
+      </c>
+      <c r="I194" t="b">
+        <v>0</v>
+      </c>
+      <c r="J194" t="b">
+        <v>1</v>
+      </c>
+      <c r="K194" t="b">
+        <v>0</v>
+      </c>
+      <c r="L194" t="b">
+        <v>0</v>
+      </c>
+      <c r="M194" t="b">
+        <v>0</v>
+      </c>
+      <c r="N194" t="s">
+        <v>19</v>
+      </c>
+      <c r="P194" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16">
+      <c r="A196">
+        <v>7</v>
+      </c>
+      <c r="B196" t="s">
         <v>99</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C196" t="s">
         <v>189</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D196" t="s">
         <v>18</v>
       </c>
-      <c r="E195" t="s">
-        <v>19</v>
-      </c>
-      <c r="F195" t="s">
-        <v>19</v>
-      </c>
-      <c r="G195" t="s">
+      <c r="E196" t="s">
+        <v>19</v>
+      </c>
+      <c r="F196" t="s">
+        <v>19</v>
+      </c>
+      <c r="G196" t="s">
         <v>20</v>
       </c>
-      <c r="H195" t="b">
-        <v>1</v>
-      </c>
-      <c r="I195" t="b">
-        <v>0</v>
-      </c>
-      <c r="J195" t="b">
-        <v>1</v>
-      </c>
-      <c r="K195" t="b">
-        <v>0</v>
-      </c>
-      <c r="L195" t="b">
-        <v>0</v>
-      </c>
-      <c r="M195" t="b">
-        <v>0</v>
-      </c>
-      <c r="N195" t="s">
+      <c r="H196" t="b">
+        <v>1</v>
+      </c>
+      <c r="I196" t="b">
+        <v>0</v>
+      </c>
+      <c r="J196" t="b">
+        <v>1</v>
+      </c>
+      <c r="K196" t="b">
+        <v>0</v>
+      </c>
+      <c r="L196" t="b">
+        <v>0</v>
+      </c>
+      <c r="M196" t="b">
+        <v>0</v>
+      </c>
+      <c r="N196" t="s">
         <v>21</v>
       </c>
-      <c r="O195" t="s">
+      <c r="O196" t="s">
         <v>22</v>
       </c>
-      <c r="P195" t="s">
+      <c r="P196" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="196" spans="1:16">
-      <c r="A196" t="s">
-        <v>24</v>
-      </c>
-      <c r="B196" t="s">
-        <v>24</v>
-      </c>
-      <c r="C196" t="s">
-        <v>24</v>
-      </c>
-      <c r="D196" t="s">
-        <v>191</v>
-      </c>
-      <c r="E196" t="s">
-        <v>19</v>
-      </c>
-      <c r="F196" t="s">
-        <v>19</v>
-      </c>
-      <c r="G196" t="s">
-        <v>91</v>
-      </c>
-      <c r="H196" t="b">
-        <v>0</v>
-      </c>
-      <c r="I196" t="b">
-        <v>0</v>
-      </c>
-      <c r="J196" t="b">
-        <v>1</v>
-      </c>
-      <c r="K196" t="b">
-        <v>0</v>
-      </c>
-      <c r="L196" t="b">
-        <v>0</v>
-      </c>
-      <c r="M196" t="b">
-        <v>0</v>
-      </c>
-      <c r="N196" t="s">
-        <v>19</v>
-      </c>
-      <c r="P196" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="197" spans="1:16">
@@ -8777,22 +8774,22 @@
         <v>24</v>
       </c>
       <c r="D197" t="s">
-        <v>138</v>
-      </c>
-      <c r="E197">
-        <v>0</v>
-      </c>
-      <c r="F197">
+        <v>158</v>
+      </c>
+      <c r="E197" t="s">
+        <v>19</v>
+      </c>
+      <c r="F197" t="s">
         <v>19</v>
       </c>
       <c r="G197" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="H197" t="b">
         <v>0</v>
       </c>
       <c r="I197" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J197" t="b">
         <v>1</v>
@@ -8807,7 +8804,7 @@
         <v>0</v>
       </c>
       <c r="N197" t="s">
-        <v>136</v>
+        <v>21</v>
       </c>
       <c r="P197" t="s">
         <v>24</v>
@@ -8824,7 +8821,7 @@
         <v>24</v>
       </c>
       <c r="D198" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="E198" t="s">
         <v>19</v>
@@ -8854,74 +8851,77 @@
         <v>0</v>
       </c>
       <c r="N198" t="s">
+        <v>19</v>
+      </c>
+      <c r="P198" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16">
+      <c r="A200">
+        <v>7</v>
+      </c>
+      <c r="B200" t="s">
+        <v>53</v>
+      </c>
+      <c r="C200" t="s">
+        <v>191</v>
+      </c>
+      <c r="D200" t="s">
+        <v>18</v>
+      </c>
+      <c r="E200" t="s">
+        <v>19</v>
+      </c>
+      <c r="F200" t="s">
+        <v>19</v>
+      </c>
+      <c r="G200" t="s">
+        <v>20</v>
+      </c>
+      <c r="H200" t="b">
+        <v>1</v>
+      </c>
+      <c r="I200" t="b">
+        <v>0</v>
+      </c>
+      <c r="J200" t="b">
+        <v>1</v>
+      </c>
+      <c r="K200" t="b">
+        <v>0</v>
+      </c>
+      <c r="L200" t="b">
+        <v>0</v>
+      </c>
+      <c r="M200" t="b">
+        <v>0</v>
+      </c>
+      <c r="N200" t="s">
         <v>21</v>
       </c>
-      <c r="P198" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="199" spans="1:16">
-      <c r="A199" t="s">
-        <v>24</v>
-      </c>
-      <c r="B199" t="s">
-        <v>24</v>
-      </c>
-      <c r="C199" t="s">
-        <v>24</v>
-      </c>
-      <c r="D199" t="s">
-        <v>187</v>
-      </c>
-      <c r="E199" t="s">
-        <v>19</v>
-      </c>
-      <c r="F199" t="s">
-        <v>19</v>
-      </c>
-      <c r="G199" t="s">
-        <v>20</v>
-      </c>
-      <c r="H199" t="b">
-        <v>0</v>
-      </c>
-      <c r="I199" t="b">
-        <v>1</v>
-      </c>
-      <c r="J199" t="b">
-        <v>1</v>
-      </c>
-      <c r="K199" t="b">
-        <v>0</v>
-      </c>
-      <c r="L199" t="b">
-        <v>0</v>
-      </c>
-      <c r="M199" t="b">
-        <v>0</v>
-      </c>
-      <c r="N199" t="s">
-        <v>19</v>
-      </c>
-      <c r="P199" t="s">
-        <v>24</v>
+      <c r="O200" t="s">
+        <v>22</v>
+      </c>
+      <c r="P200" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="201" spans="1:16">
-      <c r="A201">
-        <v>7</v>
+      <c r="A201" t="s">
+        <v>24</v>
       </c>
       <c r="B201" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C201" t="s">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="D201" t="s">
-        <v>18</v>
-      </c>
-      <c r="E201" t="s">
-        <v>19</v>
+        <v>193</v>
+      </c>
+      <c r="E201">
+        <v>0</v>
       </c>
       <c r="F201" t="s">
         <v>19</v>
@@ -8930,7 +8930,7 @@
         <v>20</v>
       </c>
       <c r="H201" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I201" t="b">
         <v>0</v>
@@ -8948,13 +8948,10 @@
         <v>0</v>
       </c>
       <c r="N201" t="s">
-        <v>21</v>
-      </c>
-      <c r="O201" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P201" t="s">
-        <v>193</v>
+        <v>24</v>
       </c>
     </row>
     <row r="202" spans="1:16">
@@ -8970,14 +8967,14 @@
       <c r="D202" t="s">
         <v>194</v>
       </c>
-      <c r="E202">
-        <v>0</v>
+      <c r="E202" t="s">
+        <v>19</v>
       </c>
       <c r="F202" t="s">
         <v>19</v>
       </c>
       <c r="G202" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="H202" t="b">
         <v>0</v>
@@ -9015,7 +9012,7 @@
         <v>24</v>
       </c>
       <c r="D203" t="s">
-        <v>195</v>
+        <v>111</v>
       </c>
       <c r="E203" t="s">
         <v>19</v>
@@ -9024,13 +9021,13 @@
         <v>19</v>
       </c>
       <c r="G203" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="H203" t="b">
         <v>0</v>
       </c>
       <c r="I203" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J203" t="b">
         <v>1</v>
@@ -9062,7 +9059,7 @@
         <v>24</v>
       </c>
       <c r="D204" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E204" t="s">
         <v>19</v>
@@ -9109,7 +9106,7 @@
         <v>24</v>
       </c>
       <c r="D205" t="s">
-        <v>115</v>
+        <v>195</v>
       </c>
       <c r="E205" t="s">
         <v>19</v>
@@ -9156,7 +9153,7 @@
         <v>24</v>
       </c>
       <c r="D206" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="E206" t="s">
         <v>19</v>
@@ -9174,68 +9171,21 @@
         <v>1</v>
       </c>
       <c r="J206" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L206" t="b">
         <v>0</v>
       </c>
       <c r="M206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N206" t="s">
         <v>19</v>
       </c>
       <c r="P206" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="207" spans="1:16">
-      <c r="A207" t="s">
-        <v>24</v>
-      </c>
-      <c r="B207" t="s">
-        <v>24</v>
-      </c>
-      <c r="C207" t="s">
-        <v>24</v>
-      </c>
-      <c r="D207" t="s">
-        <v>158</v>
-      </c>
-      <c r="E207" t="s">
-        <v>19</v>
-      </c>
-      <c r="F207" t="s">
-        <v>19</v>
-      </c>
-      <c r="G207" t="s">
-        <v>20</v>
-      </c>
-      <c r="H207" t="b">
-        <v>0</v>
-      </c>
-      <c r="I207" t="b">
-        <v>1</v>
-      </c>
-      <c r="J207" t="b">
-        <v>0</v>
-      </c>
-      <c r="K207" t="b">
-        <v>1</v>
-      </c>
-      <c r="L207" t="b">
-        <v>0</v>
-      </c>
-      <c r="M207" t="b">
-        <v>1</v>
-      </c>
-      <c r="N207" t="s">
-        <v>19</v>
-      </c>
-      <c r="P207" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>